<commit_message>
some changes to avoid nodes
view simulate traffic function to know more
</commit_message>
<xml_diff>
--- a/traffic_incident.xlsx
+++ b/traffic_incident.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,33 +458,33 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Roadwork</t>
+          <t>Vehicle breakdown</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1.33635140407453</v>
+        <v>1.366393554102729</v>
       </c>
       <c r="C2" t="n">
-        <v>103.9795047198802</v>
+        <v>103.7091049793846</v>
       </c>
       <c r="D2" t="n">
-        <v>139735890</v>
+        <v>158067840</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Vehicle breakdown</t>
+          <t>Roadwork</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1.437220848790937</v>
+        <v>1.344872523694638</v>
       </c>
       <c r="C3" t="n">
-        <v>103.7684627703709</v>
+        <v>103.8008012700982</v>
       </c>
       <c r="D3" t="n">
-        <v>157992135</v>
+        <v>139655796</v>
       </c>
     </row>
     <row r="4">
@@ -494,13 +494,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1.295590034878018</v>
+        <v>1.33635140407453</v>
       </c>
       <c r="C4" t="n">
-        <v>103.8924287199076</v>
+        <v>103.9795047198802</v>
       </c>
       <c r="D4" t="n">
-        <v>1143824826</v>
+        <v>139735890</v>
       </c>
     </row>
     <row r="5">
@@ -510,13 +510,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1.435415770128466</v>
+        <v>1.295590034878018</v>
       </c>
       <c r="C5" t="n">
-        <v>103.7685725486829</v>
+        <v>103.8924287199076</v>
       </c>
       <c r="D5" t="n">
-        <v>158016522</v>
+        <v>1143824826</v>
       </c>
     </row>
     <row r="6">
@@ -526,13 +526,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1.329643461681577</v>
+        <v>1.399175873917032</v>
       </c>
       <c r="C6" t="n">
-        <v>103.8445527705207</v>
+        <v>103.7738428336265</v>
       </c>
       <c r="D6" t="n">
-        <v>886297460</v>
+        <v>5272416387</v>
       </c>
     </row>
     <row r="7">
@@ -542,13 +542,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1.399175873917032</v>
+        <v>1.331731353207238</v>
       </c>
       <c r="C7" t="n">
-        <v>103.7738428336265</v>
+        <v>103.8177332088875</v>
       </c>
       <c r="D7" t="n">
-        <v>5272416387</v>
+        <v>241595350</v>
       </c>
     </row>
     <row r="8">
@@ -558,61 +558,61 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1.331731353207238</v>
+        <v>1.395202988681009</v>
       </c>
       <c r="C8" t="n">
-        <v>103.8177332088875</v>
+        <v>103.8168103182145</v>
       </c>
       <c r="D8" t="n">
-        <v>241595350</v>
+        <v>148992996</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Roadwork</t>
+          <t>Heavy Traffic</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1.395202988681009</v>
+        <v>1.343493280384666</v>
       </c>
       <c r="C9" t="n">
-        <v>103.8168103182145</v>
+        <v>103.6418624407713</v>
       </c>
       <c r="D9" t="n">
-        <v>148992996</v>
+        <v>148133968</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Heavy Traffic</t>
+          <t>Roadwork</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1.332430492341808</v>
+        <v>1.40114503416915</v>
       </c>
       <c r="C10" t="n">
-        <v>103.8625444822982</v>
+        <v>103.87235047762</v>
       </c>
       <c r="D10" t="n">
-        <v>250326976</v>
+        <v>3636481276</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Heavy Traffic</t>
+          <t>Roadwork</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1.343493280384666</v>
+        <v>1.368615011940697</v>
       </c>
       <c r="C11" t="n">
-        <v>103.6418624407713</v>
+        <v>103.7162652832473</v>
       </c>
       <c r="D11" t="n">
-        <v>148133968</v>
+        <v>158067818</v>
       </c>
     </row>
     <row r="12">
@@ -622,13 +622,13 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1.34032722429001</v>
+        <v>1.348217635145913</v>
       </c>
       <c r="C12" t="n">
-        <v>103.8051185574835</v>
+        <v>103.9549179861231</v>
       </c>
       <c r="D12" t="n">
-        <v>139655727</v>
+        <v>627795097</v>
       </c>
     </row>
     <row r="13">
@@ -638,13 +638,13 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1.401350645866867</v>
+        <v>1.34895197238415</v>
       </c>
       <c r="C13" t="n">
-        <v>103.8795132487888</v>
+        <v>103.6934238369014</v>
       </c>
       <c r="D13" t="n">
-        <v>6169983452</v>
+        <v>567939404</v>
       </c>
     </row>
     <row r="14">
@@ -654,13 +654,13 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1.368615011940697</v>
+        <v>1.360914211975437</v>
       </c>
       <c r="C14" t="n">
-        <v>103.7162652832473</v>
+        <v>103.9610319873716</v>
       </c>
       <c r="D14" t="n">
-        <v>158067818</v>
+        <v>6323597084</v>
       </c>
     </row>
     <row r="15">
@@ -670,13 +670,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1.348217635145913</v>
+        <v>1.378417484619901</v>
       </c>
       <c r="C15" t="n">
-        <v>103.9549179861231</v>
+        <v>103.9238304190541</v>
       </c>
       <c r="D15" t="n">
-        <v>627795097</v>
+        <v>135080726</v>
       </c>
     </row>
     <row r="16">
@@ -686,13 +686,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1.34895197238415</v>
+        <v>1.342822808856306</v>
       </c>
       <c r="C16" t="n">
-        <v>103.6934238369014</v>
+        <v>103.7466255047426</v>
       </c>
       <c r="D16" t="n">
-        <v>567939404</v>
+        <v>1218588051</v>
       </c>
     </row>
     <row r="17">
@@ -702,13 +702,13 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1.360914211975437</v>
+        <v>1.347892723763722</v>
       </c>
       <c r="C17" t="n">
-        <v>103.9610319873716</v>
+        <v>103.9543987729199</v>
       </c>
       <c r="D17" t="n">
-        <v>6323597084</v>
+        <v>137481616</v>
       </c>
     </row>
     <row r="18">
@@ -718,13 +718,13 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1.378417484619901</v>
+        <v>1.354145196935542</v>
       </c>
       <c r="C18" t="n">
-        <v>103.9238304190541</v>
+        <v>103.7272496538722</v>
       </c>
       <c r="D18" t="n">
-        <v>135080726</v>
+        <v>139672081</v>
       </c>
     </row>
     <row r="19">
@@ -734,13 +734,13 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>1.342822808856306</v>
+        <v>1.389113051750533</v>
       </c>
       <c r="C19" t="n">
-        <v>103.7466255047426</v>
+        <v>103.7532970440217</v>
       </c>
       <c r="D19" t="n">
-        <v>1218588051</v>
+        <v>158044158</v>
       </c>
     </row>
     <row r="20">
@@ -750,13 +750,13 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1.347892723763722</v>
+        <v>1.304088564346271</v>
       </c>
       <c r="C20" t="n">
-        <v>103.9543987729199</v>
+        <v>103.9194949747482</v>
       </c>
       <c r="D20" t="n">
-        <v>137481616</v>
+        <v>259758008</v>
       </c>
     </row>
     <row r="21">
@@ -766,13 +766,13 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1.354145196935542</v>
+        <v>1.355223572003486</v>
       </c>
       <c r="C21" t="n">
-        <v>103.7272496538722</v>
+        <v>103.719416471396</v>
       </c>
       <c r="D21" t="n">
-        <v>139672081</v>
+        <v>1304598696</v>
       </c>
     </row>
     <row r="22">
@@ -782,13 +782,13 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>1.389113051750533</v>
+        <v>1.355151924223111</v>
       </c>
       <c r="C22" t="n">
-        <v>103.7532970440217</v>
+        <v>103.9633934580024</v>
       </c>
       <c r="D22" t="n">
-        <v>158044158</v>
+        <v>135078416</v>
       </c>
     </row>
     <row r="23">
@@ -798,13 +798,13 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>1.304088564346271</v>
+        <v>1.301567710639741</v>
       </c>
       <c r="C23" t="n">
-        <v>103.9194949747482</v>
+        <v>103.9095384931241</v>
       </c>
       <c r="D23" t="n">
-        <v>259758008</v>
+        <v>245248320</v>
       </c>
     </row>
     <row r="24">
@@ -814,13 +814,13 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>1.355223572003486</v>
+        <v>1.292749063475387</v>
       </c>
       <c r="C24" t="n">
-        <v>103.719416471396</v>
+        <v>103.7871906402834</v>
       </c>
       <c r="D24" t="n">
-        <v>1304598696</v>
+        <v>566224199</v>
       </c>
     </row>
     <row r="25">
@@ -830,13 +830,13 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>1.355151924223111</v>
+        <v>1.356726426744445</v>
       </c>
       <c r="C25" t="n">
-        <v>103.9633934580024</v>
+        <v>103.7155388293913</v>
       </c>
       <c r="D25" t="n">
-        <v>135078416</v>
+        <v>139697312</v>
       </c>
     </row>
     <row r="26">
@@ -846,13 +846,13 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>1.301567710639741</v>
+        <v>1.362412908853572</v>
       </c>
       <c r="C26" t="n">
-        <v>103.9095384931241</v>
+        <v>103.9590366130738</v>
       </c>
       <c r="D26" t="n">
-        <v>245248320</v>
+        <v>1735669505</v>
       </c>
     </row>
     <row r="27">
@@ -862,13 +862,13 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>1.292749063475387</v>
+        <v>1.365374072663697</v>
       </c>
       <c r="C27" t="n">
-        <v>103.7871906402834</v>
+        <v>103.9539133285593</v>
       </c>
       <c r="D27" t="n">
-        <v>566224199</v>
+        <v>2857970597</v>
       </c>
     </row>
     <row r="28">
@@ -878,60 +878,12 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>1.356726426744445</v>
+        <v>1.420425919078368</v>
       </c>
       <c r="C28" t="n">
-        <v>103.7155388293913</v>
+        <v>103.7714173528471</v>
       </c>
       <c r="D28" t="n">
-        <v>139697312</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>Roadwork</t>
-        </is>
-      </c>
-      <c r="B29" t="n">
-        <v>1.362412908853572</v>
-      </c>
-      <c r="C29" t="n">
-        <v>103.9590366130738</v>
-      </c>
-      <c r="D29" t="n">
-        <v>1735669505</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>Roadwork</t>
-        </is>
-      </c>
-      <c r="B30" t="n">
-        <v>1.365374072663697</v>
-      </c>
-      <c r="C30" t="n">
-        <v>103.9539133285593</v>
-      </c>
-      <c r="D30" t="n">
-        <v>2857970597</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>Roadwork</t>
-        </is>
-      </c>
-      <c r="B31" t="n">
-        <v>1.420425919078368</v>
-      </c>
-      <c r="C31" t="n">
-        <v>103.7714173528471</v>
-      </c>
-      <c r="D31" t="n">
         <v>1110672206</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed destination sorting issue (segment)
</commit_message>
<xml_diff>
--- a/traffic_incident.xlsx
+++ b/traffic_incident.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,13 +462,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1.379865910486545</v>
+        <v>1.324776067719318</v>
       </c>
       <c r="C2" t="n">
-        <v>103.7337854704159</v>
+        <v>103.7420009258736</v>
       </c>
       <c r="D2" t="n">
-        <v>6471702139</v>
+        <v>566531145</v>
       </c>
     </row>
     <row r="3">
@@ -478,13 +478,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1.346145630297751</v>
+        <v>1.335358592412027</v>
       </c>
       <c r="C3" t="n">
-        <v>103.7370515762182</v>
+        <v>103.7750192680982</v>
       </c>
       <c r="D3" t="n">
-        <v>6103692974</v>
+        <v>139671206</v>
       </c>
     </row>
     <row r="4">
@@ -494,29 +494,253 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1.353298000560206</v>
+        <v>1.33593426172264</v>
       </c>
       <c r="C4" t="n">
-        <v>103.6965822120331</v>
+        <v>103.8099325412368</v>
       </c>
       <c r="D4" t="n">
-        <v>567938960</v>
+        <v>392680115</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Heavy Traffic</t>
+          <t>Roadwork</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1.436920719052598</v>
+        <v>1.294540495901838</v>
       </c>
       <c r="C5" t="n">
-        <v>103.7685072682963</v>
+        <v>103.8761874369692</v>
       </c>
       <c r="D5" t="n">
-        <v>157992135</v>
+        <v>366653031</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Roadwork</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1.337821500296478</v>
+      </c>
+      <c r="C6" t="n">
+        <v>103.9805201027967</v>
+      </c>
+      <c r="D6" t="n">
+        <v>4748287569</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Roadwork</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1.313207088444847</v>
+      </c>
+      <c r="C7" t="n">
+        <v>103.9539123874291</v>
+      </c>
+      <c r="D7" t="n">
+        <v>6690114550</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Roadwork</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1.324029203005592</v>
+      </c>
+      <c r="C8" t="n">
+        <v>103.7433344949127</v>
+      </c>
+      <c r="D8" t="n">
+        <v>566531128</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Roadwork</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1.294395580676698</v>
+      </c>
+      <c r="C9" t="n">
+        <v>103.8665957683079</v>
+      </c>
+      <c r="D9" t="n">
+        <v>26782016</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Roadwork</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1.295279710111475</v>
+      </c>
+      <c r="C10" t="n">
+        <v>103.871392194302</v>
+      </c>
+      <c r="D10" t="n">
+        <v>243494149</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Roadwork</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1.292970083024035</v>
+      </c>
+      <c r="C11" t="n">
+        <v>103.8623491395152</v>
+      </c>
+      <c r="D11" t="n">
+        <v>4732339357</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Roadwork</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1.426491921158762</v>
+      </c>
+      <c r="C12" t="n">
+        <v>103.7821463731425</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1110672475</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Roadwork</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>1.329408531652229</v>
+      </c>
+      <c r="C13" t="n">
+        <v>103.846978150482</v>
+      </c>
+      <c r="D13" t="n">
+        <v>245585883</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Roadwork</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>1.395616215146429</v>
+      </c>
+      <c r="C14" t="n">
+        <v>103.8576328064338</v>
+      </c>
+      <c r="D14" t="n">
+        <v>5158040655</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Roadwork</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>1.304490794689495</v>
+      </c>
+      <c r="C15" t="n">
+        <v>103.770414048807</v>
+      </c>
+      <c r="D15" t="n">
+        <v>247184656</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Roadwork</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>1.408640772693746</v>
+      </c>
+      <c r="C16" t="n">
+        <v>103.8080272748565</v>
+      </c>
+      <c r="D16" t="n">
+        <v>148992674</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Roadwork</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>1.394240890722329</v>
+      </c>
+      <c r="C17" t="n">
+        <v>103.7742911599704</v>
+      </c>
+      <c r="D17" t="n">
+        <v>158014654</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Roadwork</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>1.340324439638299</v>
+      </c>
+      <c r="C18" t="n">
+        <v>103.8051868390426</v>
+      </c>
+      <c r="D18" t="n">
+        <v>139655727</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Roadwork</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1.352252843616421</v>
+      </c>
+      <c r="C19" t="n">
+        <v>103.6957155183491</v>
+      </c>
+      <c r="D19" t="n">
+        <v>567939126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
retrieved speedband from LTA api for original route
</commit_message>
<xml_diff>
--- a/traffic_incident.xlsx
+++ b/traffic_incident.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,17 +458,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Accident</t>
+          <t>Vehicle breakdown</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1.440491672265059</v>
+        <v>1.424653170043902</v>
       </c>
       <c r="C2" t="n">
-        <v>103.76829249273</v>
+        <v>103.7910440091601</v>
       </c>
       <c r="D2" t="n">
-        <v>1884349939</v>
+        <v>440588376</v>
       </c>
     </row>
     <row r="3">
@@ -478,13 +478,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1.330328271085954</v>
+        <v>1.329566083085618</v>
       </c>
       <c r="C3" t="n">
-        <v>103.9152015923327</v>
+        <v>103.8398779449462</v>
       </c>
       <c r="D3" t="n">
-        <v>1849458129</v>
+        <v>1223810685</v>
       </c>
     </row>
     <row r="4">
@@ -494,13 +494,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1.309615816817113</v>
+        <v>1.294395580676698</v>
       </c>
       <c r="C4" t="n">
-        <v>103.8757620402856</v>
+        <v>103.8665957683079</v>
       </c>
       <c r="D4" t="n">
-        <v>3066261840</v>
+        <v>26782016</v>
       </c>
     </row>
     <row r="5">
@@ -510,13 +510,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1.300410885561765</v>
+        <v>1.383978872974393</v>
       </c>
       <c r="C5" t="n">
-        <v>103.8779458712998</v>
+        <v>103.9187785015995</v>
       </c>
       <c r="D5" t="n">
-        <v>1637064322</v>
+        <v>5726683755</v>
       </c>
     </row>
     <row r="6">
@@ -526,13 +526,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1.270873380297158</v>
+        <v>1.399693726009656</v>
       </c>
       <c r="C6" t="n">
-        <v>103.8565719413897</v>
+        <v>103.8580241805984</v>
       </c>
       <c r="D6" t="n">
-        <v>5006326691</v>
+        <v>1781710554</v>
       </c>
     </row>
     <row r="7">
@@ -542,13 +542,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1.270311527891478</v>
+        <v>1.329431928728425</v>
       </c>
       <c r="C7" t="n">
-        <v>103.8582452413363</v>
+        <v>103.8583187295057</v>
       </c>
       <c r="D7" t="n">
-        <v>5006326691</v>
+        <v>250830816</v>
       </c>
     </row>
     <row r="8">
@@ -558,13 +558,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1.395616215146429</v>
+        <v>1.390077478097602</v>
       </c>
       <c r="C8" t="n">
-        <v>103.8576328064338</v>
+        <v>103.7465491295866</v>
       </c>
       <c r="D8" t="n">
-        <v>5158040655</v>
+        <v>1734061685</v>
       </c>
     </row>
     <row r="9">
@@ -574,13 +574,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1.298178361107145</v>
+        <v>1.388890087119251</v>
       </c>
       <c r="C9" t="n">
-        <v>103.8003640080351</v>
+        <v>103.7578528352893</v>
       </c>
       <c r="D9" t="n">
-        <v>247331373</v>
+        <v>5045819346</v>
       </c>
     </row>
     <row r="10">
@@ -590,13 +590,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1.354265709309715</v>
+        <v>1.4008676440462</v>
       </c>
       <c r="C10" t="n">
-        <v>103.9005297935488</v>
+        <v>103.8597329453334</v>
       </c>
       <c r="D10" t="n">
-        <v>370010176</v>
+        <v>1781710559</v>
       </c>
     </row>
     <row r="11">
@@ -606,13 +606,13 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1.333070893064765</v>
+        <v>1.387215261909439</v>
       </c>
       <c r="C11" t="n">
-        <v>103.8890100726651</v>
+        <v>103.7562256569732</v>
       </c>
       <c r="D11" t="n">
-        <v>239833041</v>
+        <v>236726630</v>
       </c>
     </row>
     <row r="12">
@@ -622,13 +622,13 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1.329863864471722</v>
+        <v>1.330328271085954</v>
       </c>
       <c r="C12" t="n">
-        <v>103.8445306580607</v>
+        <v>103.9152015923327</v>
       </c>
       <c r="D12" t="n">
-        <v>886297460</v>
+        <v>1849458129</v>
       </c>
     </row>
     <row r="13">
@@ -638,13 +638,13 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1.280904538002612</v>
+        <v>1.309615816817113</v>
       </c>
       <c r="C13" t="n">
-        <v>103.8746779618057</v>
+        <v>103.8757620402856</v>
       </c>
       <c r="D13" t="n">
-        <v>6938787891</v>
+        <v>3066261840</v>
       </c>
     </row>
     <row r="14">
@@ -654,13 +654,13 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1.335214775723557</v>
+        <v>1.300410885561765</v>
       </c>
       <c r="C14" t="n">
-        <v>103.861906736975</v>
+        <v>103.8779458712998</v>
       </c>
       <c r="D14" t="n">
-        <v>137302917</v>
+        <v>1637064322</v>
       </c>
     </row>
     <row r="15">
@@ -670,13 +670,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1.325673028980316</v>
+        <v>1.395616215146429</v>
       </c>
       <c r="C15" t="n">
-        <v>103.7406708548471</v>
+        <v>103.8576328064338</v>
       </c>
       <c r="D15" t="n">
-        <v>1350302489</v>
+        <v>5158040655</v>
       </c>
     </row>
     <row r="16">
@@ -686,13 +686,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1.337821500296478</v>
+        <v>1.298178361107145</v>
       </c>
       <c r="C16" t="n">
-        <v>103.9805201027967</v>
+        <v>103.8003640080351</v>
       </c>
       <c r="D16" t="n">
-        <v>4748287569</v>
+        <v>247331373</v>
       </c>
     </row>
     <row r="17">
@@ -702,13 +702,13 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1.313207088444847</v>
+        <v>1.333070893064765</v>
       </c>
       <c r="C17" t="n">
-        <v>103.9539123874291</v>
+        <v>103.8890100726651</v>
       </c>
       <c r="D17" t="n">
-        <v>6690114550</v>
+        <v>239833041</v>
       </c>
     </row>
     <row r="18">
@@ -718,13 +718,13 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1.324029203005592</v>
+        <v>1.335214775723557</v>
       </c>
       <c r="C18" t="n">
-        <v>103.7433344949127</v>
+        <v>103.861906736975</v>
       </c>
       <c r="D18" t="n">
-        <v>566531128</v>
+        <v>137302917</v>
       </c>
     </row>
     <row r="19">
@@ -734,13 +734,13 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>1.294395580676698</v>
+        <v>1.325673028980316</v>
       </c>
       <c r="C19" t="n">
-        <v>103.8665957683079</v>
+        <v>103.7406708548471</v>
       </c>
       <c r="D19" t="n">
-        <v>26782016</v>
+        <v>1350302489</v>
       </c>
     </row>
     <row r="20">
@@ -750,13 +750,13 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1.426491921158762</v>
+        <v>1.337821500296478</v>
       </c>
       <c r="C20" t="n">
-        <v>103.7821463731425</v>
+        <v>103.9805201027967</v>
       </c>
       <c r="D20" t="n">
-        <v>1110672475</v>
+        <v>4748287569</v>
       </c>
     </row>
     <row r="21">
@@ -766,13 +766,13 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1.329408531652229</v>
+        <v>1.324029203005592</v>
       </c>
       <c r="C21" t="n">
-        <v>103.846978150482</v>
+        <v>103.7433344949127</v>
       </c>
       <c r="D21" t="n">
-        <v>245585883</v>
+        <v>566531128</v>
       </c>
     </row>
     <row r="22">
@@ -782,13 +782,13 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>1.304490794689495</v>
+        <v>1.426491921158762</v>
       </c>
       <c r="C22" t="n">
-        <v>103.770414048807</v>
+        <v>103.7821463731425</v>
       </c>
       <c r="D22" t="n">
-        <v>247184656</v>
+        <v>1110672475</v>
       </c>
     </row>
     <row r="23">
@@ -798,13 +798,13 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>1.408640772693746</v>
+        <v>1.304490794689495</v>
       </c>
       <c r="C23" t="n">
-        <v>103.8080272748565</v>
+        <v>103.770414048807</v>
       </c>
       <c r="D23" t="n">
-        <v>148992674</v>
+        <v>247184656</v>
       </c>
     </row>
     <row r="24">
@@ -814,13 +814,13 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>1.394240890722329</v>
+        <v>1.408640772693746</v>
       </c>
       <c r="C24" t="n">
-        <v>103.7742911599704</v>
+        <v>103.8080272748565</v>
       </c>
       <c r="D24" t="n">
-        <v>158014654</v>
+        <v>148992674</v>
       </c>
     </row>
     <row r="25">
@@ -830,12 +830,28 @@
         </is>
       </c>
       <c r="B25" t="n">
+        <v>1.394240890722329</v>
+      </c>
+      <c r="C25" t="n">
+        <v>103.7742911599704</v>
+      </c>
+      <c r="D25" t="n">
+        <v>158014654</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Roadwork</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
         <v>1.352252843616421</v>
       </c>
-      <c r="C25" t="n">
+      <c r="C26" t="n">
         <v>103.6957155183491</v>
       </c>
-      <c r="D25" t="n">
+      <c r="D26" t="n">
         <v>567939126</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Randomly select some of the traffic data entries to simulate partial live traffic flow data
</commit_message>
<xml_diff>
--- a/traffic_incident.xlsx
+++ b/traffic_incident.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D501"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -855,6 +855,2858 @@
         <v>567939126</v>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" t="inlineStr"/>
+      <c r="B27" t="inlineStr"/>
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr"/>
+      <c r="B28" t="inlineStr"/>
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr"/>
+      <c r="B29" t="inlineStr"/>
+      <c r="C29" t="inlineStr"/>
+      <c r="D29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr"/>
+      <c r="B30" t="inlineStr"/>
+      <c r="C30" t="inlineStr"/>
+      <c r="D30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr"/>
+      <c r="B31" t="inlineStr"/>
+      <c r="C31" t="inlineStr"/>
+      <c r="D31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr"/>
+      <c r="B32" t="inlineStr"/>
+      <c r="C32" t="inlineStr"/>
+      <c r="D32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr"/>
+      <c r="B33" t="inlineStr"/>
+      <c r="C33" t="inlineStr"/>
+      <c r="D33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr"/>
+      <c r="B34" t="inlineStr"/>
+      <c r="C34" t="inlineStr"/>
+      <c r="D34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr"/>
+      <c r="B35" t="inlineStr"/>
+      <c r="C35" t="inlineStr"/>
+      <c r="D35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr"/>
+      <c r="B36" t="inlineStr"/>
+      <c r="C36" t="inlineStr"/>
+      <c r="D36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr"/>
+      <c r="B37" t="inlineStr"/>
+      <c r="C37" t="inlineStr"/>
+      <c r="D37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr"/>
+      <c r="B38" t="inlineStr"/>
+      <c r="C38" t="inlineStr"/>
+      <c r="D38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr"/>
+      <c r="B39" t="inlineStr"/>
+      <c r="C39" t="inlineStr"/>
+      <c r="D39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr"/>
+      <c r="B40" t="inlineStr"/>
+      <c r="C40" t="inlineStr"/>
+      <c r="D40" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr"/>
+      <c r="B41" t="inlineStr"/>
+      <c r="C41" t="inlineStr"/>
+      <c r="D41" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr"/>
+      <c r="B42" t="inlineStr"/>
+      <c r="C42" t="inlineStr"/>
+      <c r="D42" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr"/>
+      <c r="B43" t="inlineStr"/>
+      <c r="C43" t="inlineStr"/>
+      <c r="D43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr"/>
+      <c r="B44" t="inlineStr"/>
+      <c r="C44" t="inlineStr"/>
+      <c r="D44" t="inlineStr"/>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr"/>
+      <c r="B45" t="inlineStr"/>
+      <c r="C45" t="inlineStr"/>
+      <c r="D45" t="inlineStr"/>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr"/>
+      <c r="B46" t="inlineStr"/>
+      <c r="C46" t="inlineStr"/>
+      <c r="D46" t="inlineStr"/>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr"/>
+      <c r="B47" t="inlineStr"/>
+      <c r="C47" t="inlineStr"/>
+      <c r="D47" t="inlineStr"/>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr"/>
+      <c r="B48" t="inlineStr"/>
+      <c r="C48" t="inlineStr"/>
+      <c r="D48" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr"/>
+      <c r="B49" t="inlineStr"/>
+      <c r="C49" t="inlineStr"/>
+      <c r="D49" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr"/>
+      <c r="B50" t="inlineStr"/>
+      <c r="C50" t="inlineStr"/>
+      <c r="D50" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr"/>
+      <c r="B51" t="inlineStr"/>
+      <c r="C51" t="inlineStr"/>
+      <c r="D51" t="inlineStr"/>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr"/>
+      <c r="B52" t="inlineStr"/>
+      <c r="C52" t="inlineStr"/>
+      <c r="D52" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr"/>
+      <c r="B53" t="inlineStr"/>
+      <c r="C53" t="inlineStr"/>
+      <c r="D53" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr"/>
+      <c r="B54" t="inlineStr"/>
+      <c r="C54" t="inlineStr"/>
+      <c r="D54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr"/>
+      <c r="B55" t="inlineStr"/>
+      <c r="C55" t="inlineStr"/>
+      <c r="D55" t="inlineStr"/>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr"/>
+      <c r="B56" t="inlineStr"/>
+      <c r="C56" t="inlineStr"/>
+      <c r="D56" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr"/>
+      <c r="B57" t="inlineStr"/>
+      <c r="C57" t="inlineStr"/>
+      <c r="D57" t="inlineStr"/>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr"/>
+      <c r="B58" t="inlineStr"/>
+      <c r="C58" t="inlineStr"/>
+      <c r="D58" t="inlineStr"/>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr"/>
+      <c r="B59" t="inlineStr"/>
+      <c r="C59" t="inlineStr"/>
+      <c r="D59" t="inlineStr"/>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr"/>
+      <c r="B60" t="inlineStr"/>
+      <c r="C60" t="inlineStr"/>
+      <c r="D60" t="inlineStr"/>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr"/>
+      <c r="B61" t="inlineStr"/>
+      <c r="C61" t="inlineStr"/>
+      <c r="D61" t="inlineStr"/>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr"/>
+      <c r="B62" t="inlineStr"/>
+      <c r="C62" t="inlineStr"/>
+      <c r="D62" t="inlineStr"/>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr"/>
+      <c r="B63" t="inlineStr"/>
+      <c r="C63" t="inlineStr"/>
+      <c r="D63" t="inlineStr"/>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr"/>
+      <c r="B64" t="inlineStr"/>
+      <c r="C64" t="inlineStr"/>
+      <c r="D64" t="inlineStr"/>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr"/>
+      <c r="B65" t="inlineStr"/>
+      <c r="C65" t="inlineStr"/>
+      <c r="D65" t="inlineStr"/>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr"/>
+      <c r="B66" t="inlineStr"/>
+      <c r="C66" t="inlineStr"/>
+      <c r="D66" t="inlineStr"/>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr"/>
+      <c r="B67" t="inlineStr"/>
+      <c r="C67" t="inlineStr"/>
+      <c r="D67" t="inlineStr"/>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr"/>
+      <c r="B68" t="inlineStr"/>
+      <c r="C68" t="inlineStr"/>
+      <c r="D68" t="inlineStr"/>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr"/>
+      <c r="B69" t="inlineStr"/>
+      <c r="C69" t="inlineStr"/>
+      <c r="D69" t="inlineStr"/>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr"/>
+      <c r="B70" t="inlineStr"/>
+      <c r="C70" t="inlineStr"/>
+      <c r="D70" t="inlineStr"/>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr"/>
+      <c r="B71" t="inlineStr"/>
+      <c r="C71" t="inlineStr"/>
+      <c r="D71" t="inlineStr"/>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr"/>
+      <c r="B72" t="inlineStr"/>
+      <c r="C72" t="inlineStr"/>
+      <c r="D72" t="inlineStr"/>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr"/>
+      <c r="B73" t="inlineStr"/>
+      <c r="C73" t="inlineStr"/>
+      <c r="D73" t="inlineStr"/>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr"/>
+      <c r="B74" t="inlineStr"/>
+      <c r="C74" t="inlineStr"/>
+      <c r="D74" t="inlineStr"/>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr"/>
+      <c r="B75" t="inlineStr"/>
+      <c r="C75" t="inlineStr"/>
+      <c r="D75" t="inlineStr"/>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr"/>
+      <c r="B76" t="inlineStr"/>
+      <c r="C76" t="inlineStr"/>
+      <c r="D76" t="inlineStr"/>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr"/>
+      <c r="B77" t="inlineStr"/>
+      <c r="C77" t="inlineStr"/>
+      <c r="D77" t="inlineStr"/>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr"/>
+      <c r="B78" t="inlineStr"/>
+      <c r="C78" t="inlineStr"/>
+      <c r="D78" t="inlineStr"/>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr"/>
+      <c r="B79" t="inlineStr"/>
+      <c r="C79" t="inlineStr"/>
+      <c r="D79" t="inlineStr"/>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr"/>
+      <c r="B80" t="inlineStr"/>
+      <c r="C80" t="inlineStr"/>
+      <c r="D80" t="inlineStr"/>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr"/>
+      <c r="B81" t="inlineStr"/>
+      <c r="C81" t="inlineStr"/>
+      <c r="D81" t="inlineStr"/>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr"/>
+      <c r="B82" t="inlineStr"/>
+      <c r="C82" t="inlineStr"/>
+      <c r="D82" t="inlineStr"/>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr"/>
+      <c r="B83" t="inlineStr"/>
+      <c r="C83" t="inlineStr"/>
+      <c r="D83" t="inlineStr"/>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr"/>
+      <c r="B84" t="inlineStr"/>
+      <c r="C84" t="inlineStr"/>
+      <c r="D84" t="inlineStr"/>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr"/>
+      <c r="B85" t="inlineStr"/>
+      <c r="C85" t="inlineStr"/>
+      <c r="D85" t="inlineStr"/>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr"/>
+      <c r="B86" t="inlineStr"/>
+      <c r="C86" t="inlineStr"/>
+      <c r="D86" t="inlineStr"/>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr"/>
+      <c r="B87" t="inlineStr"/>
+      <c r="C87" t="inlineStr"/>
+      <c r="D87" t="inlineStr"/>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr"/>
+      <c r="B88" t="inlineStr"/>
+      <c r="C88" t="inlineStr"/>
+      <c r="D88" t="inlineStr"/>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr"/>
+      <c r="B89" t="inlineStr"/>
+      <c r="C89" t="inlineStr"/>
+      <c r="D89" t="inlineStr"/>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr"/>
+      <c r="B90" t="inlineStr"/>
+      <c r="C90" t="inlineStr"/>
+      <c r="D90" t="inlineStr"/>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr"/>
+      <c r="B91" t="inlineStr"/>
+      <c r="C91" t="inlineStr"/>
+      <c r="D91" t="inlineStr"/>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr"/>
+      <c r="B92" t="inlineStr"/>
+      <c r="C92" t="inlineStr"/>
+      <c r="D92" t="inlineStr"/>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr"/>
+      <c r="B93" t="inlineStr"/>
+      <c r="C93" t="inlineStr"/>
+      <c r="D93" t="inlineStr"/>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr"/>
+      <c r="B94" t="inlineStr"/>
+      <c r="C94" t="inlineStr"/>
+      <c r="D94" t="inlineStr"/>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr"/>
+      <c r="B95" t="inlineStr"/>
+      <c r="C95" t="inlineStr"/>
+      <c r="D95" t="inlineStr"/>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr"/>
+      <c r="B96" t="inlineStr"/>
+      <c r="C96" t="inlineStr"/>
+      <c r="D96" t="inlineStr"/>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr"/>
+      <c r="B97" t="inlineStr"/>
+      <c r="C97" t="inlineStr"/>
+      <c r="D97" t="inlineStr"/>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr"/>
+      <c r="B98" t="inlineStr"/>
+      <c r="C98" t="inlineStr"/>
+      <c r="D98" t="inlineStr"/>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr"/>
+      <c r="B99" t="inlineStr"/>
+      <c r="C99" t="inlineStr"/>
+      <c r="D99" t="inlineStr"/>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr"/>
+      <c r="B100" t="inlineStr"/>
+      <c r="C100" t="inlineStr"/>
+      <c r="D100" t="inlineStr"/>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr"/>
+      <c r="B101" t="inlineStr"/>
+      <c r="C101" t="inlineStr"/>
+      <c r="D101" t="inlineStr"/>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr"/>
+      <c r="B102" t="inlineStr"/>
+      <c r="C102" t="inlineStr"/>
+      <c r="D102" t="inlineStr"/>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr"/>
+      <c r="B103" t="inlineStr"/>
+      <c r="C103" t="inlineStr"/>
+      <c r="D103" t="inlineStr"/>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr"/>
+      <c r="B104" t="inlineStr"/>
+      <c r="C104" t="inlineStr"/>
+      <c r="D104" t="inlineStr"/>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr"/>
+      <c r="B105" t="inlineStr"/>
+      <c r="C105" t="inlineStr"/>
+      <c r="D105" t="inlineStr"/>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr"/>
+      <c r="B106" t="inlineStr"/>
+      <c r="C106" t="inlineStr"/>
+      <c r="D106" t="inlineStr"/>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr"/>
+      <c r="B107" t="inlineStr"/>
+      <c r="C107" t="inlineStr"/>
+      <c r="D107" t="inlineStr"/>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr"/>
+      <c r="B108" t="inlineStr"/>
+      <c r="C108" t="inlineStr"/>
+      <c r="D108" t="inlineStr"/>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr"/>
+      <c r="B109" t="inlineStr"/>
+      <c r="C109" t="inlineStr"/>
+      <c r="D109" t="inlineStr"/>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr"/>
+      <c r="B110" t="inlineStr"/>
+      <c r="C110" t="inlineStr"/>
+      <c r="D110" t="inlineStr"/>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr"/>
+      <c r="B111" t="inlineStr"/>
+      <c r="C111" t="inlineStr"/>
+      <c r="D111" t="inlineStr"/>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr"/>
+      <c r="B112" t="inlineStr"/>
+      <c r="C112" t="inlineStr"/>
+      <c r="D112" t="inlineStr"/>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr"/>
+      <c r="B113" t="inlineStr"/>
+      <c r="C113" t="inlineStr"/>
+      <c r="D113" t="inlineStr"/>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr"/>
+      <c r="B114" t="inlineStr"/>
+      <c r="C114" t="inlineStr"/>
+      <c r="D114" t="inlineStr"/>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr"/>
+      <c r="B115" t="inlineStr"/>
+      <c r="C115" t="inlineStr"/>
+      <c r="D115" t="inlineStr"/>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr"/>
+      <c r="B116" t="inlineStr"/>
+      <c r="C116" t="inlineStr"/>
+      <c r="D116" t="inlineStr"/>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr"/>
+      <c r="B117" t="inlineStr"/>
+      <c r="C117" t="inlineStr"/>
+      <c r="D117" t="inlineStr"/>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr"/>
+      <c r="B118" t="inlineStr"/>
+      <c r="C118" t="inlineStr"/>
+      <c r="D118" t="inlineStr"/>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr"/>
+      <c r="B119" t="inlineStr"/>
+      <c r="C119" t="inlineStr"/>
+      <c r="D119" t="inlineStr"/>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr"/>
+      <c r="B120" t="inlineStr"/>
+      <c r="C120" t="inlineStr"/>
+      <c r="D120" t="inlineStr"/>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr"/>
+      <c r="B121" t="inlineStr"/>
+      <c r="C121" t="inlineStr"/>
+      <c r="D121" t="inlineStr"/>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr"/>
+      <c r="B122" t="inlineStr"/>
+      <c r="C122" t="inlineStr"/>
+      <c r="D122" t="inlineStr"/>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr"/>
+      <c r="B123" t="inlineStr"/>
+      <c r="C123" t="inlineStr"/>
+      <c r="D123" t="inlineStr"/>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr"/>
+      <c r="B124" t="inlineStr"/>
+      <c r="C124" t="inlineStr"/>
+      <c r="D124" t="inlineStr"/>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr"/>
+      <c r="B125" t="inlineStr"/>
+      <c r="C125" t="inlineStr"/>
+      <c r="D125" t="inlineStr"/>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr"/>
+      <c r="B126" t="inlineStr"/>
+      <c r="C126" t="inlineStr"/>
+      <c r="D126" t="inlineStr"/>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr"/>
+      <c r="B127" t="inlineStr"/>
+      <c r="C127" t="inlineStr"/>
+      <c r="D127" t="inlineStr"/>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr"/>
+      <c r="B128" t="inlineStr"/>
+      <c r="C128" t="inlineStr"/>
+      <c r="D128" t="inlineStr"/>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr"/>
+      <c r="B129" t="inlineStr"/>
+      <c r="C129" t="inlineStr"/>
+      <c r="D129" t="inlineStr"/>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr"/>
+      <c r="B130" t="inlineStr"/>
+      <c r="C130" t="inlineStr"/>
+      <c r="D130" t="inlineStr"/>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr"/>
+      <c r="B131" t="inlineStr"/>
+      <c r="C131" t="inlineStr"/>
+      <c r="D131" t="inlineStr"/>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr"/>
+      <c r="B132" t="inlineStr"/>
+      <c r="C132" t="inlineStr"/>
+      <c r="D132" t="inlineStr"/>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr"/>
+      <c r="B133" t="inlineStr"/>
+      <c r="C133" t="inlineStr"/>
+      <c r="D133" t="inlineStr"/>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr"/>
+      <c r="B134" t="inlineStr"/>
+      <c r="C134" t="inlineStr"/>
+      <c r="D134" t="inlineStr"/>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr"/>
+      <c r="B135" t="inlineStr"/>
+      <c r="C135" t="inlineStr"/>
+      <c r="D135" t="inlineStr"/>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr"/>
+      <c r="B136" t="inlineStr"/>
+      <c r="C136" t="inlineStr"/>
+      <c r="D136" t="inlineStr"/>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr"/>
+      <c r="B137" t="inlineStr"/>
+      <c r="C137" t="inlineStr"/>
+      <c r="D137" t="inlineStr"/>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr"/>
+      <c r="B138" t="inlineStr"/>
+      <c r="C138" t="inlineStr"/>
+      <c r="D138" t="inlineStr"/>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr"/>
+      <c r="B139" t="inlineStr"/>
+      <c r="C139" t="inlineStr"/>
+      <c r="D139" t="inlineStr"/>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr"/>
+      <c r="B140" t="inlineStr"/>
+      <c r="C140" t="inlineStr"/>
+      <c r="D140" t="inlineStr"/>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr"/>
+      <c r="B141" t="inlineStr"/>
+      <c r="C141" t="inlineStr"/>
+      <c r="D141" t="inlineStr"/>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr"/>
+      <c r="B142" t="inlineStr"/>
+      <c r="C142" t="inlineStr"/>
+      <c r="D142" t="inlineStr"/>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr"/>
+      <c r="B143" t="inlineStr"/>
+      <c r="C143" t="inlineStr"/>
+      <c r="D143" t="inlineStr"/>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr"/>
+      <c r="B144" t="inlineStr"/>
+      <c r="C144" t="inlineStr"/>
+      <c r="D144" t="inlineStr"/>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr"/>
+      <c r="B145" t="inlineStr"/>
+      <c r="C145" t="inlineStr"/>
+      <c r="D145" t="inlineStr"/>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr"/>
+      <c r="B146" t="inlineStr"/>
+      <c r="C146" t="inlineStr"/>
+      <c r="D146" t="inlineStr"/>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr"/>
+      <c r="B147" t="inlineStr"/>
+      <c r="C147" t="inlineStr"/>
+      <c r="D147" t="inlineStr"/>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr"/>
+      <c r="B148" t="inlineStr"/>
+      <c r="C148" t="inlineStr"/>
+      <c r="D148" t="inlineStr"/>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr"/>
+      <c r="B149" t="inlineStr"/>
+      <c r="C149" t="inlineStr"/>
+      <c r="D149" t="inlineStr"/>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr"/>
+      <c r="B150" t="inlineStr"/>
+      <c r="C150" t="inlineStr"/>
+      <c r="D150" t="inlineStr"/>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr"/>
+      <c r="B151" t="inlineStr"/>
+      <c r="C151" t="inlineStr"/>
+      <c r="D151" t="inlineStr"/>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr"/>
+      <c r="B152" t="inlineStr"/>
+      <c r="C152" t="inlineStr"/>
+      <c r="D152" t="inlineStr"/>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr"/>
+      <c r="B153" t="inlineStr"/>
+      <c r="C153" t="inlineStr"/>
+      <c r="D153" t="inlineStr"/>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr"/>
+      <c r="B154" t="inlineStr"/>
+      <c r="C154" t="inlineStr"/>
+      <c r="D154" t="inlineStr"/>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr"/>
+      <c r="B155" t="inlineStr"/>
+      <c r="C155" t="inlineStr"/>
+      <c r="D155" t="inlineStr"/>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr"/>
+      <c r="B156" t="inlineStr"/>
+      <c r="C156" t="inlineStr"/>
+      <c r="D156" t="inlineStr"/>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr"/>
+      <c r="B157" t="inlineStr"/>
+      <c r="C157" t="inlineStr"/>
+      <c r="D157" t="inlineStr"/>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr"/>
+      <c r="B158" t="inlineStr"/>
+      <c r="C158" t="inlineStr"/>
+      <c r="D158" t="inlineStr"/>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr"/>
+      <c r="B159" t="inlineStr"/>
+      <c r="C159" t="inlineStr"/>
+      <c r="D159" t="inlineStr"/>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr"/>
+      <c r="B160" t="inlineStr"/>
+      <c r="C160" t="inlineStr"/>
+      <c r="D160" t="inlineStr"/>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr"/>
+      <c r="B161" t="inlineStr"/>
+      <c r="C161" t="inlineStr"/>
+      <c r="D161" t="inlineStr"/>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr"/>
+      <c r="B162" t="inlineStr"/>
+      <c r="C162" t="inlineStr"/>
+      <c r="D162" t="inlineStr"/>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr"/>
+      <c r="B163" t="inlineStr"/>
+      <c r="C163" t="inlineStr"/>
+      <c r="D163" t="inlineStr"/>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr"/>
+      <c r="B164" t="inlineStr"/>
+      <c r="C164" t="inlineStr"/>
+      <c r="D164" t="inlineStr"/>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr"/>
+      <c r="B165" t="inlineStr"/>
+      <c r="C165" t="inlineStr"/>
+      <c r="D165" t="inlineStr"/>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr"/>
+      <c r="B166" t="inlineStr"/>
+      <c r="C166" t="inlineStr"/>
+      <c r="D166" t="inlineStr"/>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr"/>
+      <c r="B167" t="inlineStr"/>
+      <c r="C167" t="inlineStr"/>
+      <c r="D167" t="inlineStr"/>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr"/>
+      <c r="B168" t="inlineStr"/>
+      <c r="C168" t="inlineStr"/>
+      <c r="D168" t="inlineStr"/>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr"/>
+      <c r="B169" t="inlineStr"/>
+      <c r="C169" t="inlineStr"/>
+      <c r="D169" t="inlineStr"/>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr"/>
+      <c r="B170" t="inlineStr"/>
+      <c r="C170" t="inlineStr"/>
+      <c r="D170" t="inlineStr"/>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr"/>
+      <c r="B171" t="inlineStr"/>
+      <c r="C171" t="inlineStr"/>
+      <c r="D171" t="inlineStr"/>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr"/>
+      <c r="B172" t="inlineStr"/>
+      <c r="C172" t="inlineStr"/>
+      <c r="D172" t="inlineStr"/>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr"/>
+      <c r="B173" t="inlineStr"/>
+      <c r="C173" t="inlineStr"/>
+      <c r="D173" t="inlineStr"/>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr"/>
+      <c r="B174" t="inlineStr"/>
+      <c r="C174" t="inlineStr"/>
+      <c r="D174" t="inlineStr"/>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr"/>
+      <c r="B175" t="inlineStr"/>
+      <c r="C175" t="inlineStr"/>
+      <c r="D175" t="inlineStr"/>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr"/>
+      <c r="B176" t="inlineStr"/>
+      <c r="C176" t="inlineStr"/>
+      <c r="D176" t="inlineStr"/>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr"/>
+      <c r="B177" t="inlineStr"/>
+      <c r="C177" t="inlineStr"/>
+      <c r="D177" t="inlineStr"/>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr"/>
+      <c r="B178" t="inlineStr"/>
+      <c r="C178" t="inlineStr"/>
+      <c r="D178" t="inlineStr"/>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr"/>
+      <c r="B179" t="inlineStr"/>
+      <c r="C179" t="inlineStr"/>
+      <c r="D179" t="inlineStr"/>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr"/>
+      <c r="B180" t="inlineStr"/>
+      <c r="C180" t="inlineStr"/>
+      <c r="D180" t="inlineStr"/>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr"/>
+      <c r="B181" t="inlineStr"/>
+      <c r="C181" t="inlineStr"/>
+      <c r="D181" t="inlineStr"/>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr"/>
+      <c r="B182" t="inlineStr"/>
+      <c r="C182" t="inlineStr"/>
+      <c r="D182" t="inlineStr"/>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr"/>
+      <c r="B183" t="inlineStr"/>
+      <c r="C183" t="inlineStr"/>
+      <c r="D183" t="inlineStr"/>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr"/>
+      <c r="B184" t="inlineStr"/>
+      <c r="C184" t="inlineStr"/>
+      <c r="D184" t="inlineStr"/>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr"/>
+      <c r="B185" t="inlineStr"/>
+      <c r="C185" t="inlineStr"/>
+      <c r="D185" t="inlineStr"/>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr"/>
+      <c r="B186" t="inlineStr"/>
+      <c r="C186" t="inlineStr"/>
+      <c r="D186" t="inlineStr"/>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr"/>
+      <c r="B187" t="inlineStr"/>
+      <c r="C187" t="inlineStr"/>
+      <c r="D187" t="inlineStr"/>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr"/>
+      <c r="B188" t="inlineStr"/>
+      <c r="C188" t="inlineStr"/>
+      <c r="D188" t="inlineStr"/>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr"/>
+      <c r="B189" t="inlineStr"/>
+      <c r="C189" t="inlineStr"/>
+      <c r="D189" t="inlineStr"/>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr"/>
+      <c r="B190" t="inlineStr"/>
+      <c r="C190" t="inlineStr"/>
+      <c r="D190" t="inlineStr"/>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr"/>
+      <c r="B191" t="inlineStr"/>
+      <c r="C191" t="inlineStr"/>
+      <c r="D191" t="inlineStr"/>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr"/>
+      <c r="B192" t="inlineStr"/>
+      <c r="C192" t="inlineStr"/>
+      <c r="D192" t="inlineStr"/>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr"/>
+      <c r="B193" t="inlineStr"/>
+      <c r="C193" t="inlineStr"/>
+      <c r="D193" t="inlineStr"/>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr"/>
+      <c r="B194" t="inlineStr"/>
+      <c r="C194" t="inlineStr"/>
+      <c r="D194" t="inlineStr"/>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr"/>
+      <c r="B195" t="inlineStr"/>
+      <c r="C195" t="inlineStr"/>
+      <c r="D195" t="inlineStr"/>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr"/>
+      <c r="B196" t="inlineStr"/>
+      <c r="C196" t="inlineStr"/>
+      <c r="D196" t="inlineStr"/>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr"/>
+      <c r="B197" t="inlineStr"/>
+      <c r="C197" t="inlineStr"/>
+      <c r="D197" t="inlineStr"/>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr"/>
+      <c r="B198" t="inlineStr"/>
+      <c r="C198" t="inlineStr"/>
+      <c r="D198" t="inlineStr"/>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr"/>
+      <c r="B199" t="inlineStr"/>
+      <c r="C199" t="inlineStr"/>
+      <c r="D199" t="inlineStr"/>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr"/>
+      <c r="B200" t="inlineStr"/>
+      <c r="C200" t="inlineStr"/>
+      <c r="D200" t="inlineStr"/>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr"/>
+      <c r="B201" t="inlineStr"/>
+      <c r="C201" t="inlineStr"/>
+      <c r="D201" t="inlineStr"/>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr"/>
+      <c r="B202" t="inlineStr"/>
+      <c r="C202" t="inlineStr"/>
+      <c r="D202" t="inlineStr"/>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr"/>
+      <c r="B203" t="inlineStr"/>
+      <c r="C203" t="inlineStr"/>
+      <c r="D203" t="inlineStr"/>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr"/>
+      <c r="B204" t="inlineStr"/>
+      <c r="C204" t="inlineStr"/>
+      <c r="D204" t="inlineStr"/>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr"/>
+      <c r="B205" t="inlineStr"/>
+      <c r="C205" t="inlineStr"/>
+      <c r="D205" t="inlineStr"/>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr"/>
+      <c r="B206" t="inlineStr"/>
+      <c r="C206" t="inlineStr"/>
+      <c r="D206" t="inlineStr"/>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr"/>
+      <c r="B207" t="inlineStr"/>
+      <c r="C207" t="inlineStr"/>
+      <c r="D207" t="inlineStr"/>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr"/>
+      <c r="B208" t="inlineStr"/>
+      <c r="C208" t="inlineStr"/>
+      <c r="D208" t="inlineStr"/>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr"/>
+      <c r="B209" t="inlineStr"/>
+      <c r="C209" t="inlineStr"/>
+      <c r="D209" t="inlineStr"/>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr"/>
+      <c r="B210" t="inlineStr"/>
+      <c r="C210" t="inlineStr"/>
+      <c r="D210" t="inlineStr"/>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr"/>
+      <c r="B211" t="inlineStr"/>
+      <c r="C211" t="inlineStr"/>
+      <c r="D211" t="inlineStr"/>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr"/>
+      <c r="B212" t="inlineStr"/>
+      <c r="C212" t="inlineStr"/>
+      <c r="D212" t="inlineStr"/>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr"/>
+      <c r="B213" t="inlineStr"/>
+      <c r="C213" t="inlineStr"/>
+      <c r="D213" t="inlineStr"/>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr"/>
+      <c r="B214" t="inlineStr"/>
+      <c r="C214" t="inlineStr"/>
+      <c r="D214" t="inlineStr"/>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr"/>
+      <c r="B215" t="inlineStr"/>
+      <c r="C215" t="inlineStr"/>
+      <c r="D215" t="inlineStr"/>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr"/>
+      <c r="B216" t="inlineStr"/>
+      <c r="C216" t="inlineStr"/>
+      <c r="D216" t="inlineStr"/>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr"/>
+      <c r="B217" t="inlineStr"/>
+      <c r="C217" t="inlineStr"/>
+      <c r="D217" t="inlineStr"/>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr"/>
+      <c r="B218" t="inlineStr"/>
+      <c r="C218" t="inlineStr"/>
+      <c r="D218" t="inlineStr"/>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr"/>
+      <c r="B219" t="inlineStr"/>
+      <c r="C219" t="inlineStr"/>
+      <c r="D219" t="inlineStr"/>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr"/>
+      <c r="B220" t="inlineStr"/>
+      <c r="C220" t="inlineStr"/>
+      <c r="D220" t="inlineStr"/>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr"/>
+      <c r="B221" t="inlineStr"/>
+      <c r="C221" t="inlineStr"/>
+      <c r="D221" t="inlineStr"/>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr"/>
+      <c r="B222" t="inlineStr"/>
+      <c r="C222" t="inlineStr"/>
+      <c r="D222" t="inlineStr"/>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr"/>
+      <c r="B223" t="inlineStr"/>
+      <c r="C223" t="inlineStr"/>
+      <c r="D223" t="inlineStr"/>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr"/>
+      <c r="B224" t="inlineStr"/>
+      <c r="C224" t="inlineStr"/>
+      <c r="D224" t="inlineStr"/>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr"/>
+      <c r="B225" t="inlineStr"/>
+      <c r="C225" t="inlineStr"/>
+      <c r="D225" t="inlineStr"/>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr"/>
+      <c r="B226" t="inlineStr"/>
+      <c r="C226" t="inlineStr"/>
+      <c r="D226" t="inlineStr"/>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr"/>
+      <c r="B227" t="inlineStr"/>
+      <c r="C227" t="inlineStr"/>
+      <c r="D227" t="inlineStr"/>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr"/>
+      <c r="B228" t="inlineStr"/>
+      <c r="C228" t="inlineStr"/>
+      <c r="D228" t="inlineStr"/>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr"/>
+      <c r="B229" t="inlineStr"/>
+      <c r="C229" t="inlineStr"/>
+      <c r="D229" t="inlineStr"/>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr"/>
+      <c r="B230" t="inlineStr"/>
+      <c r="C230" t="inlineStr"/>
+      <c r="D230" t="inlineStr"/>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr"/>
+      <c r="B231" t="inlineStr"/>
+      <c r="C231" t="inlineStr"/>
+      <c r="D231" t="inlineStr"/>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr"/>
+      <c r="B232" t="inlineStr"/>
+      <c r="C232" t="inlineStr"/>
+      <c r="D232" t="inlineStr"/>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr"/>
+      <c r="B233" t="inlineStr"/>
+      <c r="C233" t="inlineStr"/>
+      <c r="D233" t="inlineStr"/>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr"/>
+      <c r="B234" t="inlineStr"/>
+      <c r="C234" t="inlineStr"/>
+      <c r="D234" t="inlineStr"/>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr"/>
+      <c r="B235" t="inlineStr"/>
+      <c r="C235" t="inlineStr"/>
+      <c r="D235" t="inlineStr"/>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr"/>
+      <c r="B236" t="inlineStr"/>
+      <c r="C236" t="inlineStr"/>
+      <c r="D236" t="inlineStr"/>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr"/>
+      <c r="B237" t="inlineStr"/>
+      <c r="C237" t="inlineStr"/>
+      <c r="D237" t="inlineStr"/>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr"/>
+      <c r="B238" t="inlineStr"/>
+      <c r="C238" t="inlineStr"/>
+      <c r="D238" t="inlineStr"/>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr"/>
+      <c r="B239" t="inlineStr"/>
+      <c r="C239" t="inlineStr"/>
+      <c r="D239" t="inlineStr"/>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr"/>
+      <c r="B240" t="inlineStr"/>
+      <c r="C240" t="inlineStr"/>
+      <c r="D240" t="inlineStr"/>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr"/>
+      <c r="B241" t="inlineStr"/>
+      <c r="C241" t="inlineStr"/>
+      <c r="D241" t="inlineStr"/>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr"/>
+      <c r="B242" t="inlineStr"/>
+      <c r="C242" t="inlineStr"/>
+      <c r="D242" t="inlineStr"/>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr"/>
+      <c r="B243" t="inlineStr"/>
+      <c r="C243" t="inlineStr"/>
+      <c r="D243" t="inlineStr"/>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr"/>
+      <c r="B244" t="inlineStr"/>
+      <c r="C244" t="inlineStr"/>
+      <c r="D244" t="inlineStr"/>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr"/>
+      <c r="B245" t="inlineStr"/>
+      <c r="C245" t="inlineStr"/>
+      <c r="D245" t="inlineStr"/>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr"/>
+      <c r="B246" t="inlineStr"/>
+      <c r="C246" t="inlineStr"/>
+      <c r="D246" t="inlineStr"/>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr"/>
+      <c r="B247" t="inlineStr"/>
+      <c r="C247" t="inlineStr"/>
+      <c r="D247" t="inlineStr"/>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr"/>
+      <c r="B248" t="inlineStr"/>
+      <c r="C248" t="inlineStr"/>
+      <c r="D248" t="inlineStr"/>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr"/>
+      <c r="B249" t="inlineStr"/>
+      <c r="C249" t="inlineStr"/>
+      <c r="D249" t="inlineStr"/>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr"/>
+      <c r="B250" t="inlineStr"/>
+      <c r="C250" t="inlineStr"/>
+      <c r="D250" t="inlineStr"/>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr"/>
+      <c r="B251" t="inlineStr"/>
+      <c r="C251" t="inlineStr"/>
+      <c r="D251" t="inlineStr"/>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr"/>
+      <c r="B252" t="inlineStr"/>
+      <c r="C252" t="inlineStr"/>
+      <c r="D252" t="inlineStr"/>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr"/>
+      <c r="B253" t="inlineStr"/>
+      <c r="C253" t="inlineStr"/>
+      <c r="D253" t="inlineStr"/>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr"/>
+      <c r="B254" t="inlineStr"/>
+      <c r="C254" t="inlineStr"/>
+      <c r="D254" t="inlineStr"/>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr"/>
+      <c r="B255" t="inlineStr"/>
+      <c r="C255" t="inlineStr"/>
+      <c r="D255" t="inlineStr"/>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr"/>
+      <c r="B256" t="inlineStr"/>
+      <c r="C256" t="inlineStr"/>
+      <c r="D256" t="inlineStr"/>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr"/>
+      <c r="B257" t="inlineStr"/>
+      <c r="C257" t="inlineStr"/>
+      <c r="D257" t="inlineStr"/>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr"/>
+      <c r="B258" t="inlineStr"/>
+      <c r="C258" t="inlineStr"/>
+      <c r="D258" t="inlineStr"/>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr"/>
+      <c r="B259" t="inlineStr"/>
+      <c r="C259" t="inlineStr"/>
+      <c r="D259" t="inlineStr"/>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr"/>
+      <c r="B260" t="inlineStr"/>
+      <c r="C260" t="inlineStr"/>
+      <c r="D260" t="inlineStr"/>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr"/>
+      <c r="B261" t="inlineStr"/>
+      <c r="C261" t="inlineStr"/>
+      <c r="D261" t="inlineStr"/>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr"/>
+      <c r="B262" t="inlineStr"/>
+      <c r="C262" t="inlineStr"/>
+      <c r="D262" t="inlineStr"/>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr"/>
+      <c r="B263" t="inlineStr"/>
+      <c r="C263" t="inlineStr"/>
+      <c r="D263" t="inlineStr"/>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr"/>
+      <c r="B264" t="inlineStr"/>
+      <c r="C264" t="inlineStr"/>
+      <c r="D264" t="inlineStr"/>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr"/>
+      <c r="B265" t="inlineStr"/>
+      <c r="C265" t="inlineStr"/>
+      <c r="D265" t="inlineStr"/>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr"/>
+      <c r="B266" t="inlineStr"/>
+      <c r="C266" t="inlineStr"/>
+      <c r="D266" t="inlineStr"/>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr"/>
+      <c r="B267" t="inlineStr"/>
+      <c r="C267" t="inlineStr"/>
+      <c r="D267" t="inlineStr"/>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr"/>
+      <c r="B268" t="inlineStr"/>
+      <c r="C268" t="inlineStr"/>
+      <c r="D268" t="inlineStr"/>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr"/>
+      <c r="B269" t="inlineStr"/>
+      <c r="C269" t="inlineStr"/>
+      <c r="D269" t="inlineStr"/>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr"/>
+      <c r="B270" t="inlineStr"/>
+      <c r="C270" t="inlineStr"/>
+      <c r="D270" t="inlineStr"/>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr"/>
+      <c r="B271" t="inlineStr"/>
+      <c r="C271" t="inlineStr"/>
+      <c r="D271" t="inlineStr"/>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr"/>
+      <c r="B272" t="inlineStr"/>
+      <c r="C272" t="inlineStr"/>
+      <c r="D272" t="inlineStr"/>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr"/>
+      <c r="B273" t="inlineStr"/>
+      <c r="C273" t="inlineStr"/>
+      <c r="D273" t="inlineStr"/>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr"/>
+      <c r="B274" t="inlineStr"/>
+      <c r="C274" t="inlineStr"/>
+      <c r="D274" t="inlineStr"/>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr"/>
+      <c r="B275" t="inlineStr"/>
+      <c r="C275" t="inlineStr"/>
+      <c r="D275" t="inlineStr"/>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr"/>
+      <c r="B276" t="inlineStr"/>
+      <c r="C276" t="inlineStr"/>
+      <c r="D276" t="inlineStr"/>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr"/>
+      <c r="B277" t="inlineStr"/>
+      <c r="C277" t="inlineStr"/>
+      <c r="D277" t="inlineStr"/>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr"/>
+      <c r="B278" t="inlineStr"/>
+      <c r="C278" t="inlineStr"/>
+      <c r="D278" t="inlineStr"/>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr"/>
+      <c r="B279" t="inlineStr"/>
+      <c r="C279" t="inlineStr"/>
+      <c r="D279" t="inlineStr"/>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr"/>
+      <c r="B280" t="inlineStr"/>
+      <c r="C280" t="inlineStr"/>
+      <c r="D280" t="inlineStr"/>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr"/>
+      <c r="B281" t="inlineStr"/>
+      <c r="C281" t="inlineStr"/>
+      <c r="D281" t="inlineStr"/>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr"/>
+      <c r="B282" t="inlineStr"/>
+      <c r="C282" t="inlineStr"/>
+      <c r="D282" t="inlineStr"/>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr"/>
+      <c r="B283" t="inlineStr"/>
+      <c r="C283" t="inlineStr"/>
+      <c r="D283" t="inlineStr"/>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr"/>
+      <c r="B284" t="inlineStr"/>
+      <c r="C284" t="inlineStr"/>
+      <c r="D284" t="inlineStr"/>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr"/>
+      <c r="B285" t="inlineStr"/>
+      <c r="C285" t="inlineStr"/>
+      <c r="D285" t="inlineStr"/>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr"/>
+      <c r="B286" t="inlineStr"/>
+      <c r="C286" t="inlineStr"/>
+      <c r="D286" t="inlineStr"/>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr"/>
+      <c r="B287" t="inlineStr"/>
+      <c r="C287" t="inlineStr"/>
+      <c r="D287" t="inlineStr"/>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr"/>
+      <c r="B288" t="inlineStr"/>
+      <c r="C288" t="inlineStr"/>
+      <c r="D288" t="inlineStr"/>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr"/>
+      <c r="B289" t="inlineStr"/>
+      <c r="C289" t="inlineStr"/>
+      <c r="D289" t="inlineStr"/>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr"/>
+      <c r="B290" t="inlineStr"/>
+      <c r="C290" t="inlineStr"/>
+      <c r="D290" t="inlineStr"/>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr"/>
+      <c r="B291" t="inlineStr"/>
+      <c r="C291" t="inlineStr"/>
+      <c r="D291" t="inlineStr"/>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr"/>
+      <c r="B292" t="inlineStr"/>
+      <c r="C292" t="inlineStr"/>
+      <c r="D292" t="inlineStr"/>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr"/>
+      <c r="B293" t="inlineStr"/>
+      <c r="C293" t="inlineStr"/>
+      <c r="D293" t="inlineStr"/>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr"/>
+      <c r="B294" t="inlineStr"/>
+      <c r="C294" t="inlineStr"/>
+      <c r="D294" t="inlineStr"/>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr"/>
+      <c r="B295" t="inlineStr"/>
+      <c r="C295" t="inlineStr"/>
+      <c r="D295" t="inlineStr"/>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr"/>
+      <c r="B296" t="inlineStr"/>
+      <c r="C296" t="inlineStr"/>
+      <c r="D296" t="inlineStr"/>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr"/>
+      <c r="B297" t="inlineStr"/>
+      <c r="C297" t="inlineStr"/>
+      <c r="D297" t="inlineStr"/>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr"/>
+      <c r="B298" t="inlineStr"/>
+      <c r="C298" t="inlineStr"/>
+      <c r="D298" t="inlineStr"/>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr"/>
+      <c r="B299" t="inlineStr"/>
+      <c r="C299" t="inlineStr"/>
+      <c r="D299" t="inlineStr"/>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr"/>
+      <c r="B300" t="inlineStr"/>
+      <c r="C300" t="inlineStr"/>
+      <c r="D300" t="inlineStr"/>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr"/>
+      <c r="B301" t="inlineStr"/>
+      <c r="C301" t="inlineStr"/>
+      <c r="D301" t="inlineStr"/>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr"/>
+      <c r="B302" t="inlineStr"/>
+      <c r="C302" t="inlineStr"/>
+      <c r="D302" t="inlineStr"/>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr"/>
+      <c r="B303" t="inlineStr"/>
+      <c r="C303" t="inlineStr"/>
+      <c r="D303" t="inlineStr"/>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr"/>
+      <c r="B304" t="inlineStr"/>
+      <c r="C304" t="inlineStr"/>
+      <c r="D304" t="inlineStr"/>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr"/>
+      <c r="B305" t="inlineStr"/>
+      <c r="C305" t="inlineStr"/>
+      <c r="D305" t="inlineStr"/>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr"/>
+      <c r="B306" t="inlineStr"/>
+      <c r="C306" t="inlineStr"/>
+      <c r="D306" t="inlineStr"/>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr"/>
+      <c r="B307" t="inlineStr"/>
+      <c r="C307" t="inlineStr"/>
+      <c r="D307" t="inlineStr"/>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr"/>
+      <c r="B308" t="inlineStr"/>
+      <c r="C308" t="inlineStr"/>
+      <c r="D308" t="inlineStr"/>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr"/>
+      <c r="B309" t="inlineStr"/>
+      <c r="C309" t="inlineStr"/>
+      <c r="D309" t="inlineStr"/>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr"/>
+      <c r="B310" t="inlineStr"/>
+      <c r="C310" t="inlineStr"/>
+      <c r="D310" t="inlineStr"/>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr"/>
+      <c r="B311" t="inlineStr"/>
+      <c r="C311" t="inlineStr"/>
+      <c r="D311" t="inlineStr"/>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr"/>
+      <c r="B312" t="inlineStr"/>
+      <c r="C312" t="inlineStr"/>
+      <c r="D312" t="inlineStr"/>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr"/>
+      <c r="B313" t="inlineStr"/>
+      <c r="C313" t="inlineStr"/>
+      <c r="D313" t="inlineStr"/>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr"/>
+      <c r="B314" t="inlineStr"/>
+      <c r="C314" t="inlineStr"/>
+      <c r="D314" t="inlineStr"/>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr"/>
+      <c r="B315" t="inlineStr"/>
+      <c r="C315" t="inlineStr"/>
+      <c r="D315" t="inlineStr"/>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr"/>
+      <c r="B316" t="inlineStr"/>
+      <c r="C316" t="inlineStr"/>
+      <c r="D316" t="inlineStr"/>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr"/>
+      <c r="B317" t="inlineStr"/>
+      <c r="C317" t="inlineStr"/>
+      <c r="D317" t="inlineStr"/>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr"/>
+      <c r="B318" t="inlineStr"/>
+      <c r="C318" t="inlineStr"/>
+      <c r="D318" t="inlineStr"/>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr"/>
+      <c r="B319" t="inlineStr"/>
+      <c r="C319" t="inlineStr"/>
+      <c r="D319" t="inlineStr"/>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr"/>
+      <c r="B320" t="inlineStr"/>
+      <c r="C320" t="inlineStr"/>
+      <c r="D320" t="inlineStr"/>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr"/>
+      <c r="B321" t="inlineStr"/>
+      <c r="C321" t="inlineStr"/>
+      <c r="D321" t="inlineStr"/>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr"/>
+      <c r="B322" t="inlineStr"/>
+      <c r="C322" t="inlineStr"/>
+      <c r="D322" t="inlineStr"/>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr"/>
+      <c r="B323" t="inlineStr"/>
+      <c r="C323" t="inlineStr"/>
+      <c r="D323" t="inlineStr"/>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr"/>
+      <c r="B324" t="inlineStr"/>
+      <c r="C324" t="inlineStr"/>
+      <c r="D324" t="inlineStr"/>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr"/>
+      <c r="B325" t="inlineStr"/>
+      <c r="C325" t="inlineStr"/>
+      <c r="D325" t="inlineStr"/>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr"/>
+      <c r="B326" t="inlineStr"/>
+      <c r="C326" t="inlineStr"/>
+      <c r="D326" t="inlineStr"/>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr"/>
+      <c r="B327" t="inlineStr"/>
+      <c r="C327" t="inlineStr"/>
+      <c r="D327" t="inlineStr"/>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr"/>
+      <c r="B328" t="inlineStr"/>
+      <c r="C328" t="inlineStr"/>
+      <c r="D328" t="inlineStr"/>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr"/>
+      <c r="B329" t="inlineStr"/>
+      <c r="C329" t="inlineStr"/>
+      <c r="D329" t="inlineStr"/>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr"/>
+      <c r="B330" t="inlineStr"/>
+      <c r="C330" t="inlineStr"/>
+      <c r="D330" t="inlineStr"/>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr"/>
+      <c r="B331" t="inlineStr"/>
+      <c r="C331" t="inlineStr"/>
+      <c r="D331" t="inlineStr"/>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr"/>
+      <c r="B332" t="inlineStr"/>
+      <c r="C332" t="inlineStr"/>
+      <c r="D332" t="inlineStr"/>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr"/>
+      <c r="B333" t="inlineStr"/>
+      <c r="C333" t="inlineStr"/>
+      <c r="D333" t="inlineStr"/>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr"/>
+      <c r="B334" t="inlineStr"/>
+      <c r="C334" t="inlineStr"/>
+      <c r="D334" t="inlineStr"/>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr"/>
+      <c r="B335" t="inlineStr"/>
+      <c r="C335" t="inlineStr"/>
+      <c r="D335" t="inlineStr"/>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr"/>
+      <c r="B336" t="inlineStr"/>
+      <c r="C336" t="inlineStr"/>
+      <c r="D336" t="inlineStr"/>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr"/>
+      <c r="B337" t="inlineStr"/>
+      <c r="C337" t="inlineStr"/>
+      <c r="D337" t="inlineStr"/>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr"/>
+      <c r="B338" t="inlineStr"/>
+      <c r="C338" t="inlineStr"/>
+      <c r="D338" t="inlineStr"/>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr"/>
+      <c r="B339" t="inlineStr"/>
+      <c r="C339" t="inlineStr"/>
+      <c r="D339" t="inlineStr"/>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr"/>
+      <c r="B340" t="inlineStr"/>
+      <c r="C340" t="inlineStr"/>
+      <c r="D340" t="inlineStr"/>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr"/>
+      <c r="B341" t="inlineStr"/>
+      <c r="C341" t="inlineStr"/>
+      <c r="D341" t="inlineStr"/>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr"/>
+      <c r="B342" t="inlineStr"/>
+      <c r="C342" t="inlineStr"/>
+      <c r="D342" t="inlineStr"/>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr"/>
+      <c r="B343" t="inlineStr"/>
+      <c r="C343" t="inlineStr"/>
+      <c r="D343" t="inlineStr"/>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr"/>
+      <c r="B344" t="inlineStr"/>
+      <c r="C344" t="inlineStr"/>
+      <c r="D344" t="inlineStr"/>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr"/>
+      <c r="B345" t="inlineStr"/>
+      <c r="C345" t="inlineStr"/>
+      <c r="D345" t="inlineStr"/>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr"/>
+      <c r="B346" t="inlineStr"/>
+      <c r="C346" t="inlineStr"/>
+      <c r="D346" t="inlineStr"/>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr"/>
+      <c r="B347" t="inlineStr"/>
+      <c r="C347" t="inlineStr"/>
+      <c r="D347" t="inlineStr"/>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr"/>
+      <c r="B348" t="inlineStr"/>
+      <c r="C348" t="inlineStr"/>
+      <c r="D348" t="inlineStr"/>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr"/>
+      <c r="B349" t="inlineStr"/>
+      <c r="C349" t="inlineStr"/>
+      <c r="D349" t="inlineStr"/>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr"/>
+      <c r="B350" t="inlineStr"/>
+      <c r="C350" t="inlineStr"/>
+      <c r="D350" t="inlineStr"/>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr"/>
+      <c r="B351" t="inlineStr"/>
+      <c r="C351" t="inlineStr"/>
+      <c r="D351" t="inlineStr"/>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr"/>
+      <c r="B352" t="inlineStr"/>
+      <c r="C352" t="inlineStr"/>
+      <c r="D352" t="inlineStr"/>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr"/>
+      <c r="B353" t="inlineStr"/>
+      <c r="C353" t="inlineStr"/>
+      <c r="D353" t="inlineStr"/>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr"/>
+      <c r="B354" t="inlineStr"/>
+      <c r="C354" t="inlineStr"/>
+      <c r="D354" t="inlineStr"/>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr"/>
+      <c r="B355" t="inlineStr"/>
+      <c r="C355" t="inlineStr"/>
+      <c r="D355" t="inlineStr"/>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr"/>
+      <c r="B356" t="inlineStr"/>
+      <c r="C356" t="inlineStr"/>
+      <c r="D356" t="inlineStr"/>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr"/>
+      <c r="B357" t="inlineStr"/>
+      <c r="C357" t="inlineStr"/>
+      <c r="D357" t="inlineStr"/>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr"/>
+      <c r="B358" t="inlineStr"/>
+      <c r="C358" t="inlineStr"/>
+      <c r="D358" t="inlineStr"/>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr"/>
+      <c r="B359" t="inlineStr"/>
+      <c r="C359" t="inlineStr"/>
+      <c r="D359" t="inlineStr"/>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr"/>
+      <c r="B360" t="inlineStr"/>
+      <c r="C360" t="inlineStr"/>
+      <c r="D360" t="inlineStr"/>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr"/>
+      <c r="B361" t="inlineStr"/>
+      <c r="C361" t="inlineStr"/>
+      <c r="D361" t="inlineStr"/>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr"/>
+      <c r="B362" t="inlineStr"/>
+      <c r="C362" t="inlineStr"/>
+      <c r="D362" t="inlineStr"/>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr"/>
+      <c r="B363" t="inlineStr"/>
+      <c r="C363" t="inlineStr"/>
+      <c r="D363" t="inlineStr"/>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr"/>
+      <c r="B364" t="inlineStr"/>
+      <c r="C364" t="inlineStr"/>
+      <c r="D364" t="inlineStr"/>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr"/>
+      <c r="B365" t="inlineStr"/>
+      <c r="C365" t="inlineStr"/>
+      <c r="D365" t="inlineStr"/>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr"/>
+      <c r="B366" t="inlineStr"/>
+      <c r="C366" t="inlineStr"/>
+      <c r="D366" t="inlineStr"/>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr"/>
+      <c r="B367" t="inlineStr"/>
+      <c r="C367" t="inlineStr"/>
+      <c r="D367" t="inlineStr"/>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr"/>
+      <c r="B368" t="inlineStr"/>
+      <c r="C368" t="inlineStr"/>
+      <c r="D368" t="inlineStr"/>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr"/>
+      <c r="B369" t="inlineStr"/>
+      <c r="C369" t="inlineStr"/>
+      <c r="D369" t="inlineStr"/>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr"/>
+      <c r="B370" t="inlineStr"/>
+      <c r="C370" t="inlineStr"/>
+      <c r="D370" t="inlineStr"/>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr"/>
+      <c r="B371" t="inlineStr"/>
+      <c r="C371" t="inlineStr"/>
+      <c r="D371" t="inlineStr"/>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr"/>
+      <c r="B372" t="inlineStr"/>
+      <c r="C372" t="inlineStr"/>
+      <c r="D372" t="inlineStr"/>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr"/>
+      <c r="B373" t="inlineStr"/>
+      <c r="C373" t="inlineStr"/>
+      <c r="D373" t="inlineStr"/>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr"/>
+      <c r="B374" t="inlineStr"/>
+      <c r="C374" t="inlineStr"/>
+      <c r="D374" t="inlineStr"/>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr"/>
+      <c r="B375" t="inlineStr"/>
+      <c r="C375" t="inlineStr"/>
+      <c r="D375" t="inlineStr"/>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr"/>
+      <c r="B376" t="inlineStr"/>
+      <c r="C376" t="inlineStr"/>
+      <c r="D376" t="inlineStr"/>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr"/>
+      <c r="B377" t="inlineStr"/>
+      <c r="C377" t="inlineStr"/>
+      <c r="D377" t="inlineStr"/>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr"/>
+      <c r="B378" t="inlineStr"/>
+      <c r="C378" t="inlineStr"/>
+      <c r="D378" t="inlineStr"/>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr"/>
+      <c r="B379" t="inlineStr"/>
+      <c r="C379" t="inlineStr"/>
+      <c r="D379" t="inlineStr"/>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr"/>
+      <c r="B380" t="inlineStr"/>
+      <c r="C380" t="inlineStr"/>
+      <c r="D380" t="inlineStr"/>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr"/>
+      <c r="B381" t="inlineStr"/>
+      <c r="C381" t="inlineStr"/>
+      <c r="D381" t="inlineStr"/>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr"/>
+      <c r="B382" t="inlineStr"/>
+      <c r="C382" t="inlineStr"/>
+      <c r="D382" t="inlineStr"/>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr"/>
+      <c r="B383" t="inlineStr"/>
+      <c r="C383" t="inlineStr"/>
+      <c r="D383" t="inlineStr"/>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr"/>
+      <c r="B384" t="inlineStr"/>
+      <c r="C384" t="inlineStr"/>
+      <c r="D384" t="inlineStr"/>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr"/>
+      <c r="B385" t="inlineStr"/>
+      <c r="C385" t="inlineStr"/>
+      <c r="D385" t="inlineStr"/>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr"/>
+      <c r="B386" t="inlineStr"/>
+      <c r="C386" t="inlineStr"/>
+      <c r="D386" t="inlineStr"/>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr"/>
+      <c r="B387" t="inlineStr"/>
+      <c r="C387" t="inlineStr"/>
+      <c r="D387" t="inlineStr"/>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr"/>
+      <c r="B388" t="inlineStr"/>
+      <c r="C388" t="inlineStr"/>
+      <c r="D388" t="inlineStr"/>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr"/>
+      <c r="B389" t="inlineStr"/>
+      <c r="C389" t="inlineStr"/>
+      <c r="D389" t="inlineStr"/>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr"/>
+      <c r="B390" t="inlineStr"/>
+      <c r="C390" t="inlineStr"/>
+      <c r="D390" t="inlineStr"/>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr"/>
+      <c r="B391" t="inlineStr"/>
+      <c r="C391" t="inlineStr"/>
+      <c r="D391" t="inlineStr"/>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr"/>
+      <c r="B392" t="inlineStr"/>
+      <c r="C392" t="inlineStr"/>
+      <c r="D392" t="inlineStr"/>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr"/>
+      <c r="B393" t="inlineStr"/>
+      <c r="C393" t="inlineStr"/>
+      <c r="D393" t="inlineStr"/>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr"/>
+      <c r="B394" t="inlineStr"/>
+      <c r="C394" t="inlineStr"/>
+      <c r="D394" t="inlineStr"/>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr"/>
+      <c r="B395" t="inlineStr"/>
+      <c r="C395" t="inlineStr"/>
+      <c r="D395" t="inlineStr"/>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr"/>
+      <c r="B396" t="inlineStr"/>
+      <c r="C396" t="inlineStr"/>
+      <c r="D396" t="inlineStr"/>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr"/>
+      <c r="B397" t="inlineStr"/>
+      <c r="C397" t="inlineStr"/>
+      <c r="D397" t="inlineStr"/>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr"/>
+      <c r="B398" t="inlineStr"/>
+      <c r="C398" t="inlineStr"/>
+      <c r="D398" t="inlineStr"/>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr"/>
+      <c r="B399" t="inlineStr"/>
+      <c r="C399" t="inlineStr"/>
+      <c r="D399" t="inlineStr"/>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr"/>
+      <c r="B400" t="inlineStr"/>
+      <c r="C400" t="inlineStr"/>
+      <c r="D400" t="inlineStr"/>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr"/>
+      <c r="B401" t="inlineStr"/>
+      <c r="C401" t="inlineStr"/>
+      <c r="D401" t="inlineStr"/>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr"/>
+      <c r="B402" t="inlineStr"/>
+      <c r="C402" t="inlineStr"/>
+      <c r="D402" t="inlineStr"/>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr"/>
+      <c r="B403" t="inlineStr"/>
+      <c r="C403" t="inlineStr"/>
+      <c r="D403" t="inlineStr"/>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr"/>
+      <c r="B404" t="inlineStr"/>
+      <c r="C404" t="inlineStr"/>
+      <c r="D404" t="inlineStr"/>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr"/>
+      <c r="B405" t="inlineStr"/>
+      <c r="C405" t="inlineStr"/>
+      <c r="D405" t="inlineStr"/>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr"/>
+      <c r="B406" t="inlineStr"/>
+      <c r="C406" t="inlineStr"/>
+      <c r="D406" t="inlineStr"/>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr"/>
+      <c r="B407" t="inlineStr"/>
+      <c r="C407" t="inlineStr"/>
+      <c r="D407" t="inlineStr"/>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr"/>
+      <c r="B408" t="inlineStr"/>
+      <c r="C408" t="inlineStr"/>
+      <c r="D408" t="inlineStr"/>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr"/>
+      <c r="B409" t="inlineStr"/>
+      <c r="C409" t="inlineStr"/>
+      <c r="D409" t="inlineStr"/>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr"/>
+      <c r="B410" t="inlineStr"/>
+      <c r="C410" t="inlineStr"/>
+      <c r="D410" t="inlineStr"/>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr"/>
+      <c r="B411" t="inlineStr"/>
+      <c r="C411" t="inlineStr"/>
+      <c r="D411" t="inlineStr"/>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr"/>
+      <c r="B412" t="inlineStr"/>
+      <c r="C412" t="inlineStr"/>
+      <c r="D412" t="inlineStr"/>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr"/>
+      <c r="B413" t="inlineStr"/>
+      <c r="C413" t="inlineStr"/>
+      <c r="D413" t="inlineStr"/>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr"/>
+      <c r="B414" t="inlineStr"/>
+      <c r="C414" t="inlineStr"/>
+      <c r="D414" t="inlineStr"/>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr"/>
+      <c r="B415" t="inlineStr"/>
+      <c r="C415" t="inlineStr"/>
+      <c r="D415" t="inlineStr"/>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr"/>
+      <c r="B416" t="inlineStr"/>
+      <c r="C416" t="inlineStr"/>
+      <c r="D416" t="inlineStr"/>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr"/>
+      <c r="B417" t="inlineStr"/>
+      <c r="C417" t="inlineStr"/>
+      <c r="D417" t="inlineStr"/>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr"/>
+      <c r="B418" t="inlineStr"/>
+      <c r="C418" t="inlineStr"/>
+      <c r="D418" t="inlineStr"/>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr"/>
+      <c r="B419" t="inlineStr"/>
+      <c r="C419" t="inlineStr"/>
+      <c r="D419" t="inlineStr"/>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr"/>
+      <c r="B420" t="inlineStr"/>
+      <c r="C420" t="inlineStr"/>
+      <c r="D420" t="inlineStr"/>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr"/>
+      <c r="B421" t="inlineStr"/>
+      <c r="C421" t="inlineStr"/>
+      <c r="D421" t="inlineStr"/>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr"/>
+      <c r="B422" t="inlineStr"/>
+      <c r="C422" t="inlineStr"/>
+      <c r="D422" t="inlineStr"/>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr"/>
+      <c r="B423" t="inlineStr"/>
+      <c r="C423" t="inlineStr"/>
+      <c r="D423" t="inlineStr"/>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr"/>
+      <c r="B424" t="inlineStr"/>
+      <c r="C424" t="inlineStr"/>
+      <c r="D424" t="inlineStr"/>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr"/>
+      <c r="B425" t="inlineStr"/>
+      <c r="C425" t="inlineStr"/>
+      <c r="D425" t="inlineStr"/>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr"/>
+      <c r="B426" t="inlineStr"/>
+      <c r="C426" t="inlineStr"/>
+      <c r="D426" t="inlineStr"/>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr"/>
+      <c r="B427" t="inlineStr"/>
+      <c r="C427" t="inlineStr"/>
+      <c r="D427" t="inlineStr"/>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr"/>
+      <c r="B428" t="inlineStr"/>
+      <c r="C428" t="inlineStr"/>
+      <c r="D428" t="inlineStr"/>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr"/>
+      <c r="B429" t="inlineStr"/>
+      <c r="C429" t="inlineStr"/>
+      <c r="D429" t="inlineStr"/>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr"/>
+      <c r="B430" t="inlineStr"/>
+      <c r="C430" t="inlineStr"/>
+      <c r="D430" t="inlineStr"/>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr"/>
+      <c r="B431" t="inlineStr"/>
+      <c r="C431" t="inlineStr"/>
+      <c r="D431" t="inlineStr"/>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr"/>
+      <c r="B432" t="inlineStr"/>
+      <c r="C432" t="inlineStr"/>
+      <c r="D432" t="inlineStr"/>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr"/>
+      <c r="B433" t="inlineStr"/>
+      <c r="C433" t="inlineStr"/>
+      <c r="D433" t="inlineStr"/>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr"/>
+      <c r="B434" t="inlineStr"/>
+      <c r="C434" t="inlineStr"/>
+      <c r="D434" t="inlineStr"/>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr"/>
+      <c r="B435" t="inlineStr"/>
+      <c r="C435" t="inlineStr"/>
+      <c r="D435" t="inlineStr"/>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr"/>
+      <c r="B436" t="inlineStr"/>
+      <c r="C436" t="inlineStr"/>
+      <c r="D436" t="inlineStr"/>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr"/>
+      <c r="B437" t="inlineStr"/>
+      <c r="C437" t="inlineStr"/>
+      <c r="D437" t="inlineStr"/>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr"/>
+      <c r="B438" t="inlineStr"/>
+      <c r="C438" t="inlineStr"/>
+      <c r="D438" t="inlineStr"/>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr"/>
+      <c r="B439" t="inlineStr"/>
+      <c r="C439" t="inlineStr"/>
+      <c r="D439" t="inlineStr"/>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr"/>
+      <c r="B440" t="inlineStr"/>
+      <c r="C440" t="inlineStr"/>
+      <c r="D440" t="inlineStr"/>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr"/>
+      <c r="B441" t="inlineStr"/>
+      <c r="C441" t="inlineStr"/>
+      <c r="D441" t="inlineStr"/>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr"/>
+      <c r="B442" t="inlineStr"/>
+      <c r="C442" t="inlineStr"/>
+      <c r="D442" t="inlineStr"/>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr"/>
+      <c r="B443" t="inlineStr"/>
+      <c r="C443" t="inlineStr"/>
+      <c r="D443" t="inlineStr"/>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr"/>
+      <c r="B444" t="inlineStr"/>
+      <c r="C444" t="inlineStr"/>
+      <c r="D444" t="inlineStr"/>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr"/>
+      <c r="B445" t="inlineStr"/>
+      <c r="C445" t="inlineStr"/>
+      <c r="D445" t="inlineStr"/>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr"/>
+      <c r="B446" t="inlineStr"/>
+      <c r="C446" t="inlineStr"/>
+      <c r="D446" t="inlineStr"/>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr"/>
+      <c r="B447" t="inlineStr"/>
+      <c r="C447" t="inlineStr"/>
+      <c r="D447" t="inlineStr"/>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr"/>
+      <c r="B448" t="inlineStr"/>
+      <c r="C448" t="inlineStr"/>
+      <c r="D448" t="inlineStr"/>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr"/>
+      <c r="B449" t="inlineStr"/>
+      <c r="C449" t="inlineStr"/>
+      <c r="D449" t="inlineStr"/>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr"/>
+      <c r="B450" t="inlineStr"/>
+      <c r="C450" t="inlineStr"/>
+      <c r="D450" t="inlineStr"/>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr"/>
+      <c r="B451" t="inlineStr"/>
+      <c r="C451" t="inlineStr"/>
+      <c r="D451" t="inlineStr"/>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr"/>
+      <c r="B452" t="inlineStr"/>
+      <c r="C452" t="inlineStr"/>
+      <c r="D452" t="inlineStr"/>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr"/>
+      <c r="B453" t="inlineStr"/>
+      <c r="C453" t="inlineStr"/>
+      <c r="D453" t="inlineStr"/>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr"/>
+      <c r="B454" t="inlineStr"/>
+      <c r="C454" t="inlineStr"/>
+      <c r="D454" t="inlineStr"/>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr"/>
+      <c r="B455" t="inlineStr"/>
+      <c r="C455" t="inlineStr"/>
+      <c r="D455" t="inlineStr"/>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr"/>
+      <c r="B456" t="inlineStr"/>
+      <c r="C456" t="inlineStr"/>
+      <c r="D456" t="inlineStr"/>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr"/>
+      <c r="B457" t="inlineStr"/>
+      <c r="C457" t="inlineStr"/>
+      <c r="D457" t="inlineStr"/>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr"/>
+      <c r="B458" t="inlineStr"/>
+      <c r="C458" t="inlineStr"/>
+      <c r="D458" t="inlineStr"/>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr"/>
+      <c r="B459" t="inlineStr"/>
+      <c r="C459" t="inlineStr"/>
+      <c r="D459" t="inlineStr"/>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr"/>
+      <c r="B460" t="inlineStr"/>
+      <c r="C460" t="inlineStr"/>
+      <c r="D460" t="inlineStr"/>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr"/>
+      <c r="B461" t="inlineStr"/>
+      <c r="C461" t="inlineStr"/>
+      <c r="D461" t="inlineStr"/>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr"/>
+      <c r="B462" t="inlineStr"/>
+      <c r="C462" t="inlineStr"/>
+      <c r="D462" t="inlineStr"/>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr"/>
+      <c r="B463" t="inlineStr"/>
+      <c r="C463" t="inlineStr"/>
+      <c r="D463" t="inlineStr"/>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr"/>
+      <c r="B464" t="inlineStr"/>
+      <c r="C464" t="inlineStr"/>
+      <c r="D464" t="inlineStr"/>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr"/>
+      <c r="B465" t="inlineStr"/>
+      <c r="C465" t="inlineStr"/>
+      <c r="D465" t="inlineStr"/>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr"/>
+      <c r="B466" t="inlineStr"/>
+      <c r="C466" t="inlineStr"/>
+      <c r="D466" t="inlineStr"/>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr"/>
+      <c r="B467" t="inlineStr"/>
+      <c r="C467" t="inlineStr"/>
+      <c r="D467" t="inlineStr"/>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr"/>
+      <c r="B468" t="inlineStr"/>
+      <c r="C468" t="inlineStr"/>
+      <c r="D468" t="inlineStr"/>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr"/>
+      <c r="B469" t="inlineStr"/>
+      <c r="C469" t="inlineStr"/>
+      <c r="D469" t="inlineStr"/>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr"/>
+      <c r="B470" t="inlineStr"/>
+      <c r="C470" t="inlineStr"/>
+      <c r="D470" t="inlineStr"/>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr"/>
+      <c r="B471" t="inlineStr"/>
+      <c r="C471" t="inlineStr"/>
+      <c r="D471" t="inlineStr"/>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr"/>
+      <c r="B472" t="inlineStr"/>
+      <c r="C472" t="inlineStr"/>
+      <c r="D472" t="inlineStr"/>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr"/>
+      <c r="B473" t="inlineStr"/>
+      <c r="C473" t="inlineStr"/>
+      <c r="D473" t="inlineStr"/>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr"/>
+      <c r="B474" t="inlineStr"/>
+      <c r="C474" t="inlineStr"/>
+      <c r="D474" t="inlineStr"/>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr"/>
+      <c r="B475" t="inlineStr"/>
+      <c r="C475" t="inlineStr"/>
+      <c r="D475" t="inlineStr"/>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr"/>
+      <c r="B476" t="inlineStr"/>
+      <c r="C476" t="inlineStr"/>
+      <c r="D476" t="inlineStr"/>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr"/>
+      <c r="B477" t="inlineStr"/>
+      <c r="C477" t="inlineStr"/>
+      <c r="D477" t="inlineStr"/>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr"/>
+      <c r="B478" t="inlineStr"/>
+      <c r="C478" t="inlineStr"/>
+      <c r="D478" t="inlineStr"/>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr"/>
+      <c r="B479" t="inlineStr"/>
+      <c r="C479" t="inlineStr"/>
+      <c r="D479" t="inlineStr"/>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr"/>
+      <c r="B480" t="inlineStr"/>
+      <c r="C480" t="inlineStr"/>
+      <c r="D480" t="inlineStr"/>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr"/>
+      <c r="B481" t="inlineStr"/>
+      <c r="C481" t="inlineStr"/>
+      <c r="D481" t="inlineStr"/>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr"/>
+      <c r="B482" t="inlineStr"/>
+      <c r="C482" t="inlineStr"/>
+      <c r="D482" t="inlineStr"/>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr"/>
+      <c r="B483" t="inlineStr"/>
+      <c r="C483" t="inlineStr"/>
+      <c r="D483" t="inlineStr"/>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr"/>
+      <c r="B484" t="inlineStr"/>
+      <c r="C484" t="inlineStr"/>
+      <c r="D484" t="inlineStr"/>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr"/>
+      <c r="B485" t="inlineStr"/>
+      <c r="C485" t="inlineStr"/>
+      <c r="D485" t="inlineStr"/>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr"/>
+      <c r="B486" t="inlineStr"/>
+      <c r="C486" t="inlineStr"/>
+      <c r="D486" t="inlineStr"/>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr"/>
+      <c r="B487" t="inlineStr"/>
+      <c r="C487" t="inlineStr"/>
+      <c r="D487" t="inlineStr"/>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr"/>
+      <c r="B488" t="inlineStr"/>
+      <c r="C488" t="inlineStr"/>
+      <c r="D488" t="inlineStr"/>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr"/>
+      <c r="B489" t="inlineStr"/>
+      <c r="C489" t="inlineStr"/>
+      <c r="D489" t="inlineStr"/>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr"/>
+      <c r="B490" t="inlineStr"/>
+      <c r="C490" t="inlineStr"/>
+      <c r="D490" t="inlineStr"/>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr"/>
+      <c r="B491" t="inlineStr"/>
+      <c r="C491" t="inlineStr"/>
+      <c r="D491" t="inlineStr"/>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr"/>
+      <c r="B492" t="inlineStr"/>
+      <c r="C492" t="inlineStr"/>
+      <c r="D492" t="inlineStr"/>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr"/>
+      <c r="B493" t="inlineStr"/>
+      <c r="C493" t="inlineStr"/>
+      <c r="D493" t="inlineStr"/>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr"/>
+      <c r="B494" t="inlineStr"/>
+      <c r="C494" t="inlineStr"/>
+      <c r="D494" t="inlineStr"/>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr"/>
+      <c r="B495" t="inlineStr"/>
+      <c r="C495" t="inlineStr"/>
+      <c r="D495" t="inlineStr"/>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr"/>
+      <c r="B496" t="inlineStr"/>
+      <c r="C496" t="inlineStr"/>
+      <c r="D496" t="inlineStr"/>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr"/>
+      <c r="B497" t="inlineStr"/>
+      <c r="C497" t="inlineStr"/>
+      <c r="D497" t="inlineStr"/>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr"/>
+      <c r="B498" t="inlineStr"/>
+      <c r="C498" t="inlineStr"/>
+      <c r="D498" t="inlineStr"/>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr"/>
+      <c r="B499" t="inlineStr"/>
+      <c r="C499" t="inlineStr"/>
+      <c r="D499" t="inlineStr"/>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr"/>
+      <c r="B500" t="inlineStr"/>
+      <c r="C500" t="inlineStr"/>
+      <c r="D500" t="inlineStr"/>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr"/>
+      <c r="B501" t="inlineStr"/>
+      <c r="C501" t="inlineStr"/>
+      <c r="D501" t="n">
+        <v>4696131095</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
just some output printing
</commit_message>
<xml_diff>
--- a/traffic_incident.xlsx
+++ b/traffic_incident.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D501"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -730,17 +730,17 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Roadwork</t>
+          <t>Heavy Traffic</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>1.356715404168217</v>
+        <v>1.294747808606078</v>
       </c>
       <c r="C19" t="n">
-        <v>103.7155715376391</v>
+        <v>103.85083927207</v>
       </c>
       <c r="D19" t="n">
-        <v>139697312</v>
+        <v>233421104</v>
       </c>
     </row>
     <row r="20">
@@ -750,29 +750,2901 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1.294747808606078</v>
+        <v>1.4369493687881</v>
       </c>
       <c r="C20" t="n">
-        <v>103.85083927207</v>
+        <v>103.7684901043165</v>
       </c>
       <c r="D20" t="n">
-        <v>233421104</v>
+        <v>157992135</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Heavy Traffic</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>1.4369493687881</v>
-      </c>
-      <c r="C21" t="n">
-        <v>103.7684901043165</v>
-      </c>
-      <c r="D21" t="n">
-        <v>157992135</v>
+      <c r="A21" t="inlineStr"/>
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr"/>
+      <c r="B22" t="inlineStr"/>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr"/>
+      <c r="B23" t="inlineStr"/>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr"/>
+      <c r="B24" t="inlineStr"/>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr"/>
+      <c r="B25" t="inlineStr"/>
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr"/>
+      <c r="B26" t="inlineStr"/>
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr"/>
+      <c r="B27" t="inlineStr"/>
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr"/>
+      <c r="B28" t="inlineStr"/>
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr"/>
+      <c r="B29" t="inlineStr"/>
+      <c r="C29" t="inlineStr"/>
+      <c r="D29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr"/>
+      <c r="B30" t="inlineStr"/>
+      <c r="C30" t="inlineStr"/>
+      <c r="D30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr"/>
+      <c r="B31" t="inlineStr"/>
+      <c r="C31" t="inlineStr"/>
+      <c r="D31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr"/>
+      <c r="B32" t="inlineStr"/>
+      <c r="C32" t="inlineStr"/>
+      <c r="D32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr"/>
+      <c r="B33" t="inlineStr"/>
+      <c r="C33" t="inlineStr"/>
+      <c r="D33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr"/>
+      <c r="B34" t="inlineStr"/>
+      <c r="C34" t="inlineStr"/>
+      <c r="D34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr"/>
+      <c r="B35" t="inlineStr"/>
+      <c r="C35" t="inlineStr"/>
+      <c r="D35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr"/>
+      <c r="B36" t="inlineStr"/>
+      <c r="C36" t="inlineStr"/>
+      <c r="D36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr"/>
+      <c r="B37" t="inlineStr"/>
+      <c r="C37" t="inlineStr"/>
+      <c r="D37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr"/>
+      <c r="B38" t="inlineStr"/>
+      <c r="C38" t="inlineStr"/>
+      <c r="D38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr"/>
+      <c r="B39" t="inlineStr"/>
+      <c r="C39" t="inlineStr"/>
+      <c r="D39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr"/>
+      <c r="B40" t="inlineStr"/>
+      <c r="C40" t="inlineStr"/>
+      <c r="D40" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr"/>
+      <c r="B41" t="inlineStr"/>
+      <c r="C41" t="inlineStr"/>
+      <c r="D41" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr"/>
+      <c r="B42" t="inlineStr"/>
+      <c r="C42" t="inlineStr"/>
+      <c r="D42" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr"/>
+      <c r="B43" t="inlineStr"/>
+      <c r="C43" t="inlineStr"/>
+      <c r="D43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr"/>
+      <c r="B44" t="inlineStr"/>
+      <c r="C44" t="inlineStr"/>
+      <c r="D44" t="inlineStr"/>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr"/>
+      <c r="B45" t="inlineStr"/>
+      <c r="C45" t="inlineStr"/>
+      <c r="D45" t="inlineStr"/>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr"/>
+      <c r="B46" t="inlineStr"/>
+      <c r="C46" t="inlineStr"/>
+      <c r="D46" t="inlineStr"/>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr"/>
+      <c r="B47" t="inlineStr"/>
+      <c r="C47" t="inlineStr"/>
+      <c r="D47" t="inlineStr"/>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr"/>
+      <c r="B48" t="inlineStr"/>
+      <c r="C48" t="inlineStr"/>
+      <c r="D48" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr"/>
+      <c r="B49" t="inlineStr"/>
+      <c r="C49" t="inlineStr"/>
+      <c r="D49" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr"/>
+      <c r="B50" t="inlineStr"/>
+      <c r="C50" t="inlineStr"/>
+      <c r="D50" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr"/>
+      <c r="B51" t="inlineStr"/>
+      <c r="C51" t="inlineStr"/>
+      <c r="D51" t="inlineStr"/>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr"/>
+      <c r="B52" t="inlineStr"/>
+      <c r="C52" t="inlineStr"/>
+      <c r="D52" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr"/>
+      <c r="B53" t="inlineStr"/>
+      <c r="C53" t="inlineStr"/>
+      <c r="D53" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr"/>
+      <c r="B54" t="inlineStr"/>
+      <c r="C54" t="inlineStr"/>
+      <c r="D54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr"/>
+      <c r="B55" t="inlineStr"/>
+      <c r="C55" t="inlineStr"/>
+      <c r="D55" t="inlineStr"/>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr"/>
+      <c r="B56" t="inlineStr"/>
+      <c r="C56" t="inlineStr"/>
+      <c r="D56" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr"/>
+      <c r="B57" t="inlineStr"/>
+      <c r="C57" t="inlineStr"/>
+      <c r="D57" t="inlineStr"/>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr"/>
+      <c r="B58" t="inlineStr"/>
+      <c r="C58" t="inlineStr"/>
+      <c r="D58" t="inlineStr"/>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr"/>
+      <c r="B59" t="inlineStr"/>
+      <c r="C59" t="inlineStr"/>
+      <c r="D59" t="inlineStr"/>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr"/>
+      <c r="B60" t="inlineStr"/>
+      <c r="C60" t="inlineStr"/>
+      <c r="D60" t="inlineStr"/>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr"/>
+      <c r="B61" t="inlineStr"/>
+      <c r="C61" t="inlineStr"/>
+      <c r="D61" t="inlineStr"/>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr"/>
+      <c r="B62" t="inlineStr"/>
+      <c r="C62" t="inlineStr"/>
+      <c r="D62" t="inlineStr"/>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr"/>
+      <c r="B63" t="inlineStr"/>
+      <c r="C63" t="inlineStr"/>
+      <c r="D63" t="inlineStr"/>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr"/>
+      <c r="B64" t="inlineStr"/>
+      <c r="C64" t="inlineStr"/>
+      <c r="D64" t="inlineStr"/>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr"/>
+      <c r="B65" t="inlineStr"/>
+      <c r="C65" t="inlineStr"/>
+      <c r="D65" t="inlineStr"/>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr"/>
+      <c r="B66" t="inlineStr"/>
+      <c r="C66" t="inlineStr"/>
+      <c r="D66" t="inlineStr"/>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr"/>
+      <c r="B67" t="inlineStr"/>
+      <c r="C67" t="inlineStr"/>
+      <c r="D67" t="inlineStr"/>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr"/>
+      <c r="B68" t="inlineStr"/>
+      <c r="C68" t="inlineStr"/>
+      <c r="D68" t="inlineStr"/>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr"/>
+      <c r="B69" t="inlineStr"/>
+      <c r="C69" t="inlineStr"/>
+      <c r="D69" t="inlineStr"/>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr"/>
+      <c r="B70" t="inlineStr"/>
+      <c r="C70" t="inlineStr"/>
+      <c r="D70" t="inlineStr"/>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr"/>
+      <c r="B71" t="inlineStr"/>
+      <c r="C71" t="inlineStr"/>
+      <c r="D71" t="inlineStr"/>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr"/>
+      <c r="B72" t="inlineStr"/>
+      <c r="C72" t="inlineStr"/>
+      <c r="D72" t="inlineStr"/>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr"/>
+      <c r="B73" t="inlineStr"/>
+      <c r="C73" t="inlineStr"/>
+      <c r="D73" t="inlineStr"/>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr"/>
+      <c r="B74" t="inlineStr"/>
+      <c r="C74" t="inlineStr"/>
+      <c r="D74" t="inlineStr"/>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr"/>
+      <c r="B75" t="inlineStr"/>
+      <c r="C75" t="inlineStr"/>
+      <c r="D75" t="inlineStr"/>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr"/>
+      <c r="B76" t="inlineStr"/>
+      <c r="C76" t="inlineStr"/>
+      <c r="D76" t="inlineStr"/>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr"/>
+      <c r="B77" t="inlineStr"/>
+      <c r="C77" t="inlineStr"/>
+      <c r="D77" t="inlineStr"/>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr"/>
+      <c r="B78" t="inlineStr"/>
+      <c r="C78" t="inlineStr"/>
+      <c r="D78" t="inlineStr"/>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr"/>
+      <c r="B79" t="inlineStr"/>
+      <c r="C79" t="inlineStr"/>
+      <c r="D79" t="inlineStr"/>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr"/>
+      <c r="B80" t="inlineStr"/>
+      <c r="C80" t="inlineStr"/>
+      <c r="D80" t="inlineStr"/>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr"/>
+      <c r="B81" t="inlineStr"/>
+      <c r="C81" t="inlineStr"/>
+      <c r="D81" t="inlineStr"/>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr"/>
+      <c r="B82" t="inlineStr"/>
+      <c r="C82" t="inlineStr"/>
+      <c r="D82" t="inlineStr"/>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr"/>
+      <c r="B83" t="inlineStr"/>
+      <c r="C83" t="inlineStr"/>
+      <c r="D83" t="inlineStr"/>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr"/>
+      <c r="B84" t="inlineStr"/>
+      <c r="C84" t="inlineStr"/>
+      <c r="D84" t="inlineStr"/>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr"/>
+      <c r="B85" t="inlineStr"/>
+      <c r="C85" t="inlineStr"/>
+      <c r="D85" t="inlineStr"/>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr"/>
+      <c r="B86" t="inlineStr"/>
+      <c r="C86" t="inlineStr"/>
+      <c r="D86" t="inlineStr"/>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr"/>
+      <c r="B87" t="inlineStr"/>
+      <c r="C87" t="inlineStr"/>
+      <c r="D87" t="inlineStr"/>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr"/>
+      <c r="B88" t="inlineStr"/>
+      <c r="C88" t="inlineStr"/>
+      <c r="D88" t="inlineStr"/>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr"/>
+      <c r="B89" t="inlineStr"/>
+      <c r="C89" t="inlineStr"/>
+      <c r="D89" t="inlineStr"/>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr"/>
+      <c r="B90" t="inlineStr"/>
+      <c r="C90" t="inlineStr"/>
+      <c r="D90" t="inlineStr"/>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr"/>
+      <c r="B91" t="inlineStr"/>
+      <c r="C91" t="inlineStr"/>
+      <c r="D91" t="inlineStr"/>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr"/>
+      <c r="B92" t="inlineStr"/>
+      <c r="C92" t="inlineStr"/>
+      <c r="D92" t="inlineStr"/>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr"/>
+      <c r="B93" t="inlineStr"/>
+      <c r="C93" t="inlineStr"/>
+      <c r="D93" t="inlineStr"/>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr"/>
+      <c r="B94" t="inlineStr"/>
+      <c r="C94" t="inlineStr"/>
+      <c r="D94" t="inlineStr"/>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr"/>
+      <c r="B95" t="inlineStr"/>
+      <c r="C95" t="inlineStr"/>
+      <c r="D95" t="inlineStr"/>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr"/>
+      <c r="B96" t="inlineStr"/>
+      <c r="C96" t="inlineStr"/>
+      <c r="D96" t="inlineStr"/>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr"/>
+      <c r="B97" t="inlineStr"/>
+      <c r="C97" t="inlineStr"/>
+      <c r="D97" t="inlineStr"/>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr"/>
+      <c r="B98" t="inlineStr"/>
+      <c r="C98" t="inlineStr"/>
+      <c r="D98" t="inlineStr"/>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr"/>
+      <c r="B99" t="inlineStr"/>
+      <c r="C99" t="inlineStr"/>
+      <c r="D99" t="inlineStr"/>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr"/>
+      <c r="B100" t="inlineStr"/>
+      <c r="C100" t="inlineStr"/>
+      <c r="D100" t="inlineStr"/>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr"/>
+      <c r="B101" t="inlineStr"/>
+      <c r="C101" t="inlineStr"/>
+      <c r="D101" t="inlineStr"/>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr"/>
+      <c r="B102" t="inlineStr"/>
+      <c r="C102" t="inlineStr"/>
+      <c r="D102" t="inlineStr"/>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr"/>
+      <c r="B103" t="inlineStr"/>
+      <c r="C103" t="inlineStr"/>
+      <c r="D103" t="inlineStr"/>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr"/>
+      <c r="B104" t="inlineStr"/>
+      <c r="C104" t="inlineStr"/>
+      <c r="D104" t="inlineStr"/>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr"/>
+      <c r="B105" t="inlineStr"/>
+      <c r="C105" t="inlineStr"/>
+      <c r="D105" t="inlineStr"/>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr"/>
+      <c r="B106" t="inlineStr"/>
+      <c r="C106" t="inlineStr"/>
+      <c r="D106" t="inlineStr"/>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr"/>
+      <c r="B107" t="inlineStr"/>
+      <c r="C107" t="inlineStr"/>
+      <c r="D107" t="inlineStr"/>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr"/>
+      <c r="B108" t="inlineStr"/>
+      <c r="C108" t="inlineStr"/>
+      <c r="D108" t="inlineStr"/>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr"/>
+      <c r="B109" t="inlineStr"/>
+      <c r="C109" t="inlineStr"/>
+      <c r="D109" t="inlineStr"/>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr"/>
+      <c r="B110" t="inlineStr"/>
+      <c r="C110" t="inlineStr"/>
+      <c r="D110" t="inlineStr"/>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr"/>
+      <c r="B111" t="inlineStr"/>
+      <c r="C111" t="inlineStr"/>
+      <c r="D111" t="inlineStr"/>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr"/>
+      <c r="B112" t="inlineStr"/>
+      <c r="C112" t="inlineStr"/>
+      <c r="D112" t="inlineStr"/>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr"/>
+      <c r="B113" t="inlineStr"/>
+      <c r="C113" t="inlineStr"/>
+      <c r="D113" t="inlineStr"/>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr"/>
+      <c r="B114" t="inlineStr"/>
+      <c r="C114" t="inlineStr"/>
+      <c r="D114" t="inlineStr"/>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr"/>
+      <c r="B115" t="inlineStr"/>
+      <c r="C115" t="inlineStr"/>
+      <c r="D115" t="inlineStr"/>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr"/>
+      <c r="B116" t="inlineStr"/>
+      <c r="C116" t="inlineStr"/>
+      <c r="D116" t="inlineStr"/>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr"/>
+      <c r="B117" t="inlineStr"/>
+      <c r="C117" t="inlineStr"/>
+      <c r="D117" t="inlineStr"/>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr"/>
+      <c r="B118" t="inlineStr"/>
+      <c r="C118" t="inlineStr"/>
+      <c r="D118" t="inlineStr"/>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr"/>
+      <c r="B119" t="inlineStr"/>
+      <c r="C119" t="inlineStr"/>
+      <c r="D119" t="inlineStr"/>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr"/>
+      <c r="B120" t="inlineStr"/>
+      <c r="C120" t="inlineStr"/>
+      <c r="D120" t="inlineStr"/>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr"/>
+      <c r="B121" t="inlineStr"/>
+      <c r="C121" t="inlineStr"/>
+      <c r="D121" t="inlineStr"/>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr"/>
+      <c r="B122" t="inlineStr"/>
+      <c r="C122" t="inlineStr"/>
+      <c r="D122" t="inlineStr"/>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr"/>
+      <c r="B123" t="inlineStr"/>
+      <c r="C123" t="inlineStr"/>
+      <c r="D123" t="inlineStr"/>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr"/>
+      <c r="B124" t="inlineStr"/>
+      <c r="C124" t="inlineStr"/>
+      <c r="D124" t="inlineStr"/>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr"/>
+      <c r="B125" t="inlineStr"/>
+      <c r="C125" t="inlineStr"/>
+      <c r="D125" t="inlineStr"/>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr"/>
+      <c r="B126" t="inlineStr"/>
+      <c r="C126" t="inlineStr"/>
+      <c r="D126" t="inlineStr"/>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr"/>
+      <c r="B127" t="inlineStr"/>
+      <c r="C127" t="inlineStr"/>
+      <c r="D127" t="inlineStr"/>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr"/>
+      <c r="B128" t="inlineStr"/>
+      <c r="C128" t="inlineStr"/>
+      <c r="D128" t="inlineStr"/>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr"/>
+      <c r="B129" t="inlineStr"/>
+      <c r="C129" t="inlineStr"/>
+      <c r="D129" t="inlineStr"/>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr"/>
+      <c r="B130" t="inlineStr"/>
+      <c r="C130" t="inlineStr"/>
+      <c r="D130" t="inlineStr"/>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr"/>
+      <c r="B131" t="inlineStr"/>
+      <c r="C131" t="inlineStr"/>
+      <c r="D131" t="inlineStr"/>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr"/>
+      <c r="B132" t="inlineStr"/>
+      <c r="C132" t="inlineStr"/>
+      <c r="D132" t="inlineStr"/>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr"/>
+      <c r="B133" t="inlineStr"/>
+      <c r="C133" t="inlineStr"/>
+      <c r="D133" t="inlineStr"/>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr"/>
+      <c r="B134" t="inlineStr"/>
+      <c r="C134" t="inlineStr"/>
+      <c r="D134" t="inlineStr"/>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr"/>
+      <c r="B135" t="inlineStr"/>
+      <c r="C135" t="inlineStr"/>
+      <c r="D135" t="inlineStr"/>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr"/>
+      <c r="B136" t="inlineStr"/>
+      <c r="C136" t="inlineStr"/>
+      <c r="D136" t="inlineStr"/>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr"/>
+      <c r="B137" t="inlineStr"/>
+      <c r="C137" t="inlineStr"/>
+      <c r="D137" t="inlineStr"/>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr"/>
+      <c r="B138" t="inlineStr"/>
+      <c r="C138" t="inlineStr"/>
+      <c r="D138" t="inlineStr"/>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr"/>
+      <c r="B139" t="inlineStr"/>
+      <c r="C139" t="inlineStr"/>
+      <c r="D139" t="inlineStr"/>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr"/>
+      <c r="B140" t="inlineStr"/>
+      <c r="C140" t="inlineStr"/>
+      <c r="D140" t="inlineStr"/>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr"/>
+      <c r="B141" t="inlineStr"/>
+      <c r="C141" t="inlineStr"/>
+      <c r="D141" t="inlineStr"/>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr"/>
+      <c r="B142" t="inlineStr"/>
+      <c r="C142" t="inlineStr"/>
+      <c r="D142" t="inlineStr"/>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr"/>
+      <c r="B143" t="inlineStr"/>
+      <c r="C143" t="inlineStr"/>
+      <c r="D143" t="inlineStr"/>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr"/>
+      <c r="B144" t="inlineStr"/>
+      <c r="C144" t="inlineStr"/>
+      <c r="D144" t="inlineStr"/>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr"/>
+      <c r="B145" t="inlineStr"/>
+      <c r="C145" t="inlineStr"/>
+      <c r="D145" t="inlineStr"/>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr"/>
+      <c r="B146" t="inlineStr"/>
+      <c r="C146" t="inlineStr"/>
+      <c r="D146" t="inlineStr"/>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr"/>
+      <c r="B147" t="inlineStr"/>
+      <c r="C147" t="inlineStr"/>
+      <c r="D147" t="inlineStr"/>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr"/>
+      <c r="B148" t="inlineStr"/>
+      <c r="C148" t="inlineStr"/>
+      <c r="D148" t="inlineStr"/>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr"/>
+      <c r="B149" t="inlineStr"/>
+      <c r="C149" t="inlineStr"/>
+      <c r="D149" t="inlineStr"/>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr"/>
+      <c r="B150" t="inlineStr"/>
+      <c r="C150" t="inlineStr"/>
+      <c r="D150" t="inlineStr"/>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr"/>
+      <c r="B151" t="inlineStr"/>
+      <c r="C151" t="inlineStr"/>
+      <c r="D151" t="inlineStr"/>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr"/>
+      <c r="B152" t="inlineStr"/>
+      <c r="C152" t="inlineStr"/>
+      <c r="D152" t="inlineStr"/>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr"/>
+      <c r="B153" t="inlineStr"/>
+      <c r="C153" t="inlineStr"/>
+      <c r="D153" t="inlineStr"/>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr"/>
+      <c r="B154" t="inlineStr"/>
+      <c r="C154" t="inlineStr"/>
+      <c r="D154" t="inlineStr"/>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr"/>
+      <c r="B155" t="inlineStr"/>
+      <c r="C155" t="inlineStr"/>
+      <c r="D155" t="inlineStr"/>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr"/>
+      <c r="B156" t="inlineStr"/>
+      <c r="C156" t="inlineStr"/>
+      <c r="D156" t="inlineStr"/>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr"/>
+      <c r="B157" t="inlineStr"/>
+      <c r="C157" t="inlineStr"/>
+      <c r="D157" t="inlineStr"/>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr"/>
+      <c r="B158" t="inlineStr"/>
+      <c r="C158" t="inlineStr"/>
+      <c r="D158" t="inlineStr"/>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr"/>
+      <c r="B159" t="inlineStr"/>
+      <c r="C159" t="inlineStr"/>
+      <c r="D159" t="inlineStr"/>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr"/>
+      <c r="B160" t="inlineStr"/>
+      <c r="C160" t="inlineStr"/>
+      <c r="D160" t="inlineStr"/>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr"/>
+      <c r="B161" t="inlineStr"/>
+      <c r="C161" t="inlineStr"/>
+      <c r="D161" t="inlineStr"/>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr"/>
+      <c r="B162" t="inlineStr"/>
+      <c r="C162" t="inlineStr"/>
+      <c r="D162" t="inlineStr"/>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr"/>
+      <c r="B163" t="inlineStr"/>
+      <c r="C163" t="inlineStr"/>
+      <c r="D163" t="inlineStr"/>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr"/>
+      <c r="B164" t="inlineStr"/>
+      <c r="C164" t="inlineStr"/>
+      <c r="D164" t="inlineStr"/>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr"/>
+      <c r="B165" t="inlineStr"/>
+      <c r="C165" t="inlineStr"/>
+      <c r="D165" t="inlineStr"/>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr"/>
+      <c r="B166" t="inlineStr"/>
+      <c r="C166" t="inlineStr"/>
+      <c r="D166" t="inlineStr"/>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr"/>
+      <c r="B167" t="inlineStr"/>
+      <c r="C167" t="inlineStr"/>
+      <c r="D167" t="inlineStr"/>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr"/>
+      <c r="B168" t="inlineStr"/>
+      <c r="C168" t="inlineStr"/>
+      <c r="D168" t="inlineStr"/>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr"/>
+      <c r="B169" t="inlineStr"/>
+      <c r="C169" t="inlineStr"/>
+      <c r="D169" t="inlineStr"/>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr"/>
+      <c r="B170" t="inlineStr"/>
+      <c r="C170" t="inlineStr"/>
+      <c r="D170" t="inlineStr"/>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr"/>
+      <c r="B171" t="inlineStr"/>
+      <c r="C171" t="inlineStr"/>
+      <c r="D171" t="inlineStr"/>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr"/>
+      <c r="B172" t="inlineStr"/>
+      <c r="C172" t="inlineStr"/>
+      <c r="D172" t="inlineStr"/>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr"/>
+      <c r="B173" t="inlineStr"/>
+      <c r="C173" t="inlineStr"/>
+      <c r="D173" t="inlineStr"/>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr"/>
+      <c r="B174" t="inlineStr"/>
+      <c r="C174" t="inlineStr"/>
+      <c r="D174" t="inlineStr"/>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr"/>
+      <c r="B175" t="inlineStr"/>
+      <c r="C175" t="inlineStr"/>
+      <c r="D175" t="inlineStr"/>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr"/>
+      <c r="B176" t="inlineStr"/>
+      <c r="C176" t="inlineStr"/>
+      <c r="D176" t="inlineStr"/>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr"/>
+      <c r="B177" t="inlineStr"/>
+      <c r="C177" t="inlineStr"/>
+      <c r="D177" t="inlineStr"/>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr"/>
+      <c r="B178" t="inlineStr"/>
+      <c r="C178" t="inlineStr"/>
+      <c r="D178" t="inlineStr"/>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr"/>
+      <c r="B179" t="inlineStr"/>
+      <c r="C179" t="inlineStr"/>
+      <c r="D179" t="inlineStr"/>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr"/>
+      <c r="B180" t="inlineStr"/>
+      <c r="C180" t="inlineStr"/>
+      <c r="D180" t="inlineStr"/>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr"/>
+      <c r="B181" t="inlineStr"/>
+      <c r="C181" t="inlineStr"/>
+      <c r="D181" t="inlineStr"/>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr"/>
+      <c r="B182" t="inlineStr"/>
+      <c r="C182" t="inlineStr"/>
+      <c r="D182" t="inlineStr"/>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr"/>
+      <c r="B183" t="inlineStr"/>
+      <c r="C183" t="inlineStr"/>
+      <c r="D183" t="inlineStr"/>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr"/>
+      <c r="B184" t="inlineStr"/>
+      <c r="C184" t="inlineStr"/>
+      <c r="D184" t="inlineStr"/>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr"/>
+      <c r="B185" t="inlineStr"/>
+      <c r="C185" t="inlineStr"/>
+      <c r="D185" t="inlineStr"/>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr"/>
+      <c r="B186" t="inlineStr"/>
+      <c r="C186" t="inlineStr"/>
+      <c r="D186" t="inlineStr"/>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr"/>
+      <c r="B187" t="inlineStr"/>
+      <c r="C187" t="inlineStr"/>
+      <c r="D187" t="inlineStr"/>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr"/>
+      <c r="B188" t="inlineStr"/>
+      <c r="C188" t="inlineStr"/>
+      <c r="D188" t="inlineStr"/>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr"/>
+      <c r="B189" t="inlineStr"/>
+      <c r="C189" t="inlineStr"/>
+      <c r="D189" t="inlineStr"/>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr"/>
+      <c r="B190" t="inlineStr"/>
+      <c r="C190" t="inlineStr"/>
+      <c r="D190" t="inlineStr"/>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr"/>
+      <c r="B191" t="inlineStr"/>
+      <c r="C191" t="inlineStr"/>
+      <c r="D191" t="inlineStr"/>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr"/>
+      <c r="B192" t="inlineStr"/>
+      <c r="C192" t="inlineStr"/>
+      <c r="D192" t="inlineStr"/>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr"/>
+      <c r="B193" t="inlineStr"/>
+      <c r="C193" t="inlineStr"/>
+      <c r="D193" t="inlineStr"/>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr"/>
+      <c r="B194" t="inlineStr"/>
+      <c r="C194" t="inlineStr"/>
+      <c r="D194" t="inlineStr"/>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr"/>
+      <c r="B195" t="inlineStr"/>
+      <c r="C195" t="inlineStr"/>
+      <c r="D195" t="inlineStr"/>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr"/>
+      <c r="B196" t="inlineStr"/>
+      <c r="C196" t="inlineStr"/>
+      <c r="D196" t="inlineStr"/>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr"/>
+      <c r="B197" t="inlineStr"/>
+      <c r="C197" t="inlineStr"/>
+      <c r="D197" t="inlineStr"/>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr"/>
+      <c r="B198" t="inlineStr"/>
+      <c r="C198" t="inlineStr"/>
+      <c r="D198" t="inlineStr"/>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr"/>
+      <c r="B199" t="inlineStr"/>
+      <c r="C199" t="inlineStr"/>
+      <c r="D199" t="inlineStr"/>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr"/>
+      <c r="B200" t="inlineStr"/>
+      <c r="C200" t="inlineStr"/>
+      <c r="D200" t="inlineStr"/>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr"/>
+      <c r="B201" t="inlineStr"/>
+      <c r="C201" t="inlineStr"/>
+      <c r="D201" t="inlineStr"/>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr"/>
+      <c r="B202" t="inlineStr"/>
+      <c r="C202" t="inlineStr"/>
+      <c r="D202" t="inlineStr"/>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr"/>
+      <c r="B203" t="inlineStr"/>
+      <c r="C203" t="inlineStr"/>
+      <c r="D203" t="inlineStr"/>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr"/>
+      <c r="B204" t="inlineStr"/>
+      <c r="C204" t="inlineStr"/>
+      <c r="D204" t="inlineStr"/>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr"/>
+      <c r="B205" t="inlineStr"/>
+      <c r="C205" t="inlineStr"/>
+      <c r="D205" t="inlineStr"/>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr"/>
+      <c r="B206" t="inlineStr"/>
+      <c r="C206" t="inlineStr"/>
+      <c r="D206" t="inlineStr"/>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr"/>
+      <c r="B207" t="inlineStr"/>
+      <c r="C207" t="inlineStr"/>
+      <c r="D207" t="inlineStr"/>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr"/>
+      <c r="B208" t="inlineStr"/>
+      <c r="C208" t="inlineStr"/>
+      <c r="D208" t="inlineStr"/>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr"/>
+      <c r="B209" t="inlineStr"/>
+      <c r="C209" t="inlineStr"/>
+      <c r="D209" t="inlineStr"/>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr"/>
+      <c r="B210" t="inlineStr"/>
+      <c r="C210" t="inlineStr"/>
+      <c r="D210" t="inlineStr"/>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr"/>
+      <c r="B211" t="inlineStr"/>
+      <c r="C211" t="inlineStr"/>
+      <c r="D211" t="inlineStr"/>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr"/>
+      <c r="B212" t="inlineStr"/>
+      <c r="C212" t="inlineStr"/>
+      <c r="D212" t="inlineStr"/>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr"/>
+      <c r="B213" t="inlineStr"/>
+      <c r="C213" t="inlineStr"/>
+      <c r="D213" t="inlineStr"/>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr"/>
+      <c r="B214" t="inlineStr"/>
+      <c r="C214" t="inlineStr"/>
+      <c r="D214" t="inlineStr"/>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr"/>
+      <c r="B215" t="inlineStr"/>
+      <c r="C215" t="inlineStr"/>
+      <c r="D215" t="inlineStr"/>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr"/>
+      <c r="B216" t="inlineStr"/>
+      <c r="C216" t="inlineStr"/>
+      <c r="D216" t="inlineStr"/>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr"/>
+      <c r="B217" t="inlineStr"/>
+      <c r="C217" t="inlineStr"/>
+      <c r="D217" t="inlineStr"/>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr"/>
+      <c r="B218" t="inlineStr"/>
+      <c r="C218" t="inlineStr"/>
+      <c r="D218" t="inlineStr"/>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr"/>
+      <c r="B219" t="inlineStr"/>
+      <c r="C219" t="inlineStr"/>
+      <c r="D219" t="inlineStr"/>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr"/>
+      <c r="B220" t="inlineStr"/>
+      <c r="C220" t="inlineStr"/>
+      <c r="D220" t="inlineStr"/>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr"/>
+      <c r="B221" t="inlineStr"/>
+      <c r="C221" t="inlineStr"/>
+      <c r="D221" t="inlineStr"/>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr"/>
+      <c r="B222" t="inlineStr"/>
+      <c r="C222" t="inlineStr"/>
+      <c r="D222" t="inlineStr"/>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr"/>
+      <c r="B223" t="inlineStr"/>
+      <c r="C223" t="inlineStr"/>
+      <c r="D223" t="inlineStr"/>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr"/>
+      <c r="B224" t="inlineStr"/>
+      <c r="C224" t="inlineStr"/>
+      <c r="D224" t="inlineStr"/>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr"/>
+      <c r="B225" t="inlineStr"/>
+      <c r="C225" t="inlineStr"/>
+      <c r="D225" t="inlineStr"/>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr"/>
+      <c r="B226" t="inlineStr"/>
+      <c r="C226" t="inlineStr"/>
+      <c r="D226" t="inlineStr"/>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr"/>
+      <c r="B227" t="inlineStr"/>
+      <c r="C227" t="inlineStr"/>
+      <c r="D227" t="inlineStr"/>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr"/>
+      <c r="B228" t="inlineStr"/>
+      <c r="C228" t="inlineStr"/>
+      <c r="D228" t="inlineStr"/>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr"/>
+      <c r="B229" t="inlineStr"/>
+      <c r="C229" t="inlineStr"/>
+      <c r="D229" t="inlineStr"/>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr"/>
+      <c r="B230" t="inlineStr"/>
+      <c r="C230" t="inlineStr"/>
+      <c r="D230" t="inlineStr"/>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr"/>
+      <c r="B231" t="inlineStr"/>
+      <c r="C231" t="inlineStr"/>
+      <c r="D231" t="inlineStr"/>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr"/>
+      <c r="B232" t="inlineStr"/>
+      <c r="C232" t="inlineStr"/>
+      <c r="D232" t="inlineStr"/>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr"/>
+      <c r="B233" t="inlineStr"/>
+      <c r="C233" t="inlineStr"/>
+      <c r="D233" t="inlineStr"/>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr"/>
+      <c r="B234" t="inlineStr"/>
+      <c r="C234" t="inlineStr"/>
+      <c r="D234" t="inlineStr"/>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr"/>
+      <c r="B235" t="inlineStr"/>
+      <c r="C235" t="inlineStr"/>
+      <c r="D235" t="inlineStr"/>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr"/>
+      <c r="B236" t="inlineStr"/>
+      <c r="C236" t="inlineStr"/>
+      <c r="D236" t="inlineStr"/>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr"/>
+      <c r="B237" t="inlineStr"/>
+      <c r="C237" t="inlineStr"/>
+      <c r="D237" t="inlineStr"/>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr"/>
+      <c r="B238" t="inlineStr"/>
+      <c r="C238" t="inlineStr"/>
+      <c r="D238" t="inlineStr"/>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr"/>
+      <c r="B239" t="inlineStr"/>
+      <c r="C239" t="inlineStr"/>
+      <c r="D239" t="inlineStr"/>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr"/>
+      <c r="B240" t="inlineStr"/>
+      <c r="C240" t="inlineStr"/>
+      <c r="D240" t="inlineStr"/>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr"/>
+      <c r="B241" t="inlineStr"/>
+      <c r="C241" t="inlineStr"/>
+      <c r="D241" t="inlineStr"/>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr"/>
+      <c r="B242" t="inlineStr"/>
+      <c r="C242" t="inlineStr"/>
+      <c r="D242" t="inlineStr"/>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr"/>
+      <c r="B243" t="inlineStr"/>
+      <c r="C243" t="inlineStr"/>
+      <c r="D243" t="inlineStr"/>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr"/>
+      <c r="B244" t="inlineStr"/>
+      <c r="C244" t="inlineStr"/>
+      <c r="D244" t="inlineStr"/>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr"/>
+      <c r="B245" t="inlineStr"/>
+      <c r="C245" t="inlineStr"/>
+      <c r="D245" t="inlineStr"/>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr"/>
+      <c r="B246" t="inlineStr"/>
+      <c r="C246" t="inlineStr"/>
+      <c r="D246" t="inlineStr"/>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr"/>
+      <c r="B247" t="inlineStr"/>
+      <c r="C247" t="inlineStr"/>
+      <c r="D247" t="inlineStr"/>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr"/>
+      <c r="B248" t="inlineStr"/>
+      <c r="C248" t="inlineStr"/>
+      <c r="D248" t="inlineStr"/>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr"/>
+      <c r="B249" t="inlineStr"/>
+      <c r="C249" t="inlineStr"/>
+      <c r="D249" t="inlineStr"/>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr"/>
+      <c r="B250" t="inlineStr"/>
+      <c r="C250" t="inlineStr"/>
+      <c r="D250" t="inlineStr"/>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr"/>
+      <c r="B251" t="inlineStr"/>
+      <c r="C251" t="inlineStr"/>
+      <c r="D251" t="inlineStr"/>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr"/>
+      <c r="B252" t="inlineStr"/>
+      <c r="C252" t="inlineStr"/>
+      <c r="D252" t="inlineStr"/>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr"/>
+      <c r="B253" t="inlineStr"/>
+      <c r="C253" t="inlineStr"/>
+      <c r="D253" t="inlineStr"/>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr"/>
+      <c r="B254" t="inlineStr"/>
+      <c r="C254" t="inlineStr"/>
+      <c r="D254" t="inlineStr"/>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr"/>
+      <c r="B255" t="inlineStr"/>
+      <c r="C255" t="inlineStr"/>
+      <c r="D255" t="inlineStr"/>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr"/>
+      <c r="B256" t="inlineStr"/>
+      <c r="C256" t="inlineStr"/>
+      <c r="D256" t="inlineStr"/>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr"/>
+      <c r="B257" t="inlineStr"/>
+      <c r="C257" t="inlineStr"/>
+      <c r="D257" t="inlineStr"/>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr"/>
+      <c r="B258" t="inlineStr"/>
+      <c r="C258" t="inlineStr"/>
+      <c r="D258" t="inlineStr"/>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr"/>
+      <c r="B259" t="inlineStr"/>
+      <c r="C259" t="inlineStr"/>
+      <c r="D259" t="inlineStr"/>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr"/>
+      <c r="B260" t="inlineStr"/>
+      <c r="C260" t="inlineStr"/>
+      <c r="D260" t="inlineStr"/>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr"/>
+      <c r="B261" t="inlineStr"/>
+      <c r="C261" t="inlineStr"/>
+      <c r="D261" t="inlineStr"/>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr"/>
+      <c r="B262" t="inlineStr"/>
+      <c r="C262" t="inlineStr"/>
+      <c r="D262" t="inlineStr"/>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr"/>
+      <c r="B263" t="inlineStr"/>
+      <c r="C263" t="inlineStr"/>
+      <c r="D263" t="inlineStr"/>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr"/>
+      <c r="B264" t="inlineStr"/>
+      <c r="C264" t="inlineStr"/>
+      <c r="D264" t="inlineStr"/>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr"/>
+      <c r="B265" t="inlineStr"/>
+      <c r="C265" t="inlineStr"/>
+      <c r="D265" t="inlineStr"/>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr"/>
+      <c r="B266" t="inlineStr"/>
+      <c r="C266" t="inlineStr"/>
+      <c r="D266" t="inlineStr"/>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr"/>
+      <c r="B267" t="inlineStr"/>
+      <c r="C267" t="inlineStr"/>
+      <c r="D267" t="inlineStr"/>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr"/>
+      <c r="B268" t="inlineStr"/>
+      <c r="C268" t="inlineStr"/>
+      <c r="D268" t="inlineStr"/>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr"/>
+      <c r="B269" t="inlineStr"/>
+      <c r="C269" t="inlineStr"/>
+      <c r="D269" t="inlineStr"/>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr"/>
+      <c r="B270" t="inlineStr"/>
+      <c r="C270" t="inlineStr"/>
+      <c r="D270" t="inlineStr"/>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr"/>
+      <c r="B271" t="inlineStr"/>
+      <c r="C271" t="inlineStr"/>
+      <c r="D271" t="inlineStr"/>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr"/>
+      <c r="B272" t="inlineStr"/>
+      <c r="C272" t="inlineStr"/>
+      <c r="D272" t="inlineStr"/>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr"/>
+      <c r="B273" t="inlineStr"/>
+      <c r="C273" t="inlineStr"/>
+      <c r="D273" t="inlineStr"/>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr"/>
+      <c r="B274" t="inlineStr"/>
+      <c r="C274" t="inlineStr"/>
+      <c r="D274" t="inlineStr"/>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr"/>
+      <c r="B275" t="inlineStr"/>
+      <c r="C275" t="inlineStr"/>
+      <c r="D275" t="inlineStr"/>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr"/>
+      <c r="B276" t="inlineStr"/>
+      <c r="C276" t="inlineStr"/>
+      <c r="D276" t="inlineStr"/>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr"/>
+      <c r="B277" t="inlineStr"/>
+      <c r="C277" t="inlineStr"/>
+      <c r="D277" t="inlineStr"/>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr"/>
+      <c r="B278" t="inlineStr"/>
+      <c r="C278" t="inlineStr"/>
+      <c r="D278" t="inlineStr"/>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr"/>
+      <c r="B279" t="inlineStr"/>
+      <c r="C279" t="inlineStr"/>
+      <c r="D279" t="inlineStr"/>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr"/>
+      <c r="B280" t="inlineStr"/>
+      <c r="C280" t="inlineStr"/>
+      <c r="D280" t="inlineStr"/>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr"/>
+      <c r="B281" t="inlineStr"/>
+      <c r="C281" t="inlineStr"/>
+      <c r="D281" t="inlineStr"/>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr"/>
+      <c r="B282" t="inlineStr"/>
+      <c r="C282" t="inlineStr"/>
+      <c r="D282" t="inlineStr"/>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr"/>
+      <c r="B283" t="inlineStr"/>
+      <c r="C283" t="inlineStr"/>
+      <c r="D283" t="inlineStr"/>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr"/>
+      <c r="B284" t="inlineStr"/>
+      <c r="C284" t="inlineStr"/>
+      <c r="D284" t="inlineStr"/>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr"/>
+      <c r="B285" t="inlineStr"/>
+      <c r="C285" t="inlineStr"/>
+      <c r="D285" t="inlineStr"/>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr"/>
+      <c r="B286" t="inlineStr"/>
+      <c r="C286" t="inlineStr"/>
+      <c r="D286" t="inlineStr"/>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr"/>
+      <c r="B287" t="inlineStr"/>
+      <c r="C287" t="inlineStr"/>
+      <c r="D287" t="inlineStr"/>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr"/>
+      <c r="B288" t="inlineStr"/>
+      <c r="C288" t="inlineStr"/>
+      <c r="D288" t="inlineStr"/>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr"/>
+      <c r="B289" t="inlineStr"/>
+      <c r="C289" t="inlineStr"/>
+      <c r="D289" t="inlineStr"/>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr"/>
+      <c r="B290" t="inlineStr"/>
+      <c r="C290" t="inlineStr"/>
+      <c r="D290" t="inlineStr"/>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr"/>
+      <c r="B291" t="inlineStr"/>
+      <c r="C291" t="inlineStr"/>
+      <c r="D291" t="inlineStr"/>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr"/>
+      <c r="B292" t="inlineStr"/>
+      <c r="C292" t="inlineStr"/>
+      <c r="D292" t="inlineStr"/>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr"/>
+      <c r="B293" t="inlineStr"/>
+      <c r="C293" t="inlineStr"/>
+      <c r="D293" t="inlineStr"/>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr"/>
+      <c r="B294" t="inlineStr"/>
+      <c r="C294" t="inlineStr"/>
+      <c r="D294" t="inlineStr"/>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr"/>
+      <c r="B295" t="inlineStr"/>
+      <c r="C295" t="inlineStr"/>
+      <c r="D295" t="inlineStr"/>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr"/>
+      <c r="B296" t="inlineStr"/>
+      <c r="C296" t="inlineStr"/>
+      <c r="D296" t="inlineStr"/>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr"/>
+      <c r="B297" t="inlineStr"/>
+      <c r="C297" t="inlineStr"/>
+      <c r="D297" t="inlineStr"/>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr"/>
+      <c r="B298" t="inlineStr"/>
+      <c r="C298" t="inlineStr"/>
+      <c r="D298" t="inlineStr"/>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr"/>
+      <c r="B299" t="inlineStr"/>
+      <c r="C299" t="inlineStr"/>
+      <c r="D299" t="inlineStr"/>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr"/>
+      <c r="B300" t="inlineStr"/>
+      <c r="C300" t="inlineStr"/>
+      <c r="D300" t="inlineStr"/>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr"/>
+      <c r="B301" t="inlineStr"/>
+      <c r="C301" t="inlineStr"/>
+      <c r="D301" t="inlineStr"/>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr"/>
+      <c r="B302" t="inlineStr"/>
+      <c r="C302" t="inlineStr"/>
+      <c r="D302" t="inlineStr"/>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr"/>
+      <c r="B303" t="inlineStr"/>
+      <c r="C303" t="inlineStr"/>
+      <c r="D303" t="inlineStr"/>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr"/>
+      <c r="B304" t="inlineStr"/>
+      <c r="C304" t="inlineStr"/>
+      <c r="D304" t="inlineStr"/>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr"/>
+      <c r="B305" t="inlineStr"/>
+      <c r="C305" t="inlineStr"/>
+      <c r="D305" t="inlineStr"/>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr"/>
+      <c r="B306" t="inlineStr"/>
+      <c r="C306" t="inlineStr"/>
+      <c r="D306" t="inlineStr"/>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr"/>
+      <c r="B307" t="inlineStr"/>
+      <c r="C307" t="inlineStr"/>
+      <c r="D307" t="inlineStr"/>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr"/>
+      <c r="B308" t="inlineStr"/>
+      <c r="C308" t="inlineStr"/>
+      <c r="D308" t="inlineStr"/>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr"/>
+      <c r="B309" t="inlineStr"/>
+      <c r="C309" t="inlineStr"/>
+      <c r="D309" t="inlineStr"/>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr"/>
+      <c r="B310" t="inlineStr"/>
+      <c r="C310" t="inlineStr"/>
+      <c r="D310" t="inlineStr"/>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr"/>
+      <c r="B311" t="inlineStr"/>
+      <c r="C311" t="inlineStr"/>
+      <c r="D311" t="inlineStr"/>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr"/>
+      <c r="B312" t="inlineStr"/>
+      <c r="C312" t="inlineStr"/>
+      <c r="D312" t="inlineStr"/>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr"/>
+      <c r="B313" t="inlineStr"/>
+      <c r="C313" t="inlineStr"/>
+      <c r="D313" t="inlineStr"/>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr"/>
+      <c r="B314" t="inlineStr"/>
+      <c r="C314" t="inlineStr"/>
+      <c r="D314" t="inlineStr"/>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr"/>
+      <c r="B315" t="inlineStr"/>
+      <c r="C315" t="inlineStr"/>
+      <c r="D315" t="inlineStr"/>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr"/>
+      <c r="B316" t="inlineStr"/>
+      <c r="C316" t="inlineStr"/>
+      <c r="D316" t="inlineStr"/>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr"/>
+      <c r="B317" t="inlineStr"/>
+      <c r="C317" t="inlineStr"/>
+      <c r="D317" t="inlineStr"/>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr"/>
+      <c r="B318" t="inlineStr"/>
+      <c r="C318" t="inlineStr"/>
+      <c r="D318" t="inlineStr"/>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr"/>
+      <c r="B319" t="inlineStr"/>
+      <c r="C319" t="inlineStr"/>
+      <c r="D319" t="inlineStr"/>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr"/>
+      <c r="B320" t="inlineStr"/>
+      <c r="C320" t="inlineStr"/>
+      <c r="D320" t="inlineStr"/>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr"/>
+      <c r="B321" t="inlineStr"/>
+      <c r="C321" t="inlineStr"/>
+      <c r="D321" t="inlineStr"/>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr"/>
+      <c r="B322" t="inlineStr"/>
+      <c r="C322" t="inlineStr"/>
+      <c r="D322" t="inlineStr"/>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr"/>
+      <c r="B323" t="inlineStr"/>
+      <c r="C323" t="inlineStr"/>
+      <c r="D323" t="inlineStr"/>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr"/>
+      <c r="B324" t="inlineStr"/>
+      <c r="C324" t="inlineStr"/>
+      <c r="D324" t="inlineStr"/>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr"/>
+      <c r="B325" t="inlineStr"/>
+      <c r="C325" t="inlineStr"/>
+      <c r="D325" t="inlineStr"/>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr"/>
+      <c r="B326" t="inlineStr"/>
+      <c r="C326" t="inlineStr"/>
+      <c r="D326" t="inlineStr"/>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr"/>
+      <c r="B327" t="inlineStr"/>
+      <c r="C327" t="inlineStr"/>
+      <c r="D327" t="inlineStr"/>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr"/>
+      <c r="B328" t="inlineStr"/>
+      <c r="C328" t="inlineStr"/>
+      <c r="D328" t="inlineStr"/>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr"/>
+      <c r="B329" t="inlineStr"/>
+      <c r="C329" t="inlineStr"/>
+      <c r="D329" t="inlineStr"/>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr"/>
+      <c r="B330" t="inlineStr"/>
+      <c r="C330" t="inlineStr"/>
+      <c r="D330" t="inlineStr"/>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr"/>
+      <c r="B331" t="inlineStr"/>
+      <c r="C331" t="inlineStr"/>
+      <c r="D331" t="inlineStr"/>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr"/>
+      <c r="B332" t="inlineStr"/>
+      <c r="C332" t="inlineStr"/>
+      <c r="D332" t="inlineStr"/>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr"/>
+      <c r="B333" t="inlineStr"/>
+      <c r="C333" t="inlineStr"/>
+      <c r="D333" t="inlineStr"/>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr"/>
+      <c r="B334" t="inlineStr"/>
+      <c r="C334" t="inlineStr"/>
+      <c r="D334" t="inlineStr"/>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr"/>
+      <c r="B335" t="inlineStr"/>
+      <c r="C335" t="inlineStr"/>
+      <c r="D335" t="inlineStr"/>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr"/>
+      <c r="B336" t="inlineStr"/>
+      <c r="C336" t="inlineStr"/>
+      <c r="D336" t="inlineStr"/>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr"/>
+      <c r="B337" t="inlineStr"/>
+      <c r="C337" t="inlineStr"/>
+      <c r="D337" t="inlineStr"/>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr"/>
+      <c r="B338" t="inlineStr"/>
+      <c r="C338" t="inlineStr"/>
+      <c r="D338" t="inlineStr"/>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr"/>
+      <c r="B339" t="inlineStr"/>
+      <c r="C339" t="inlineStr"/>
+      <c r="D339" t="inlineStr"/>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr"/>
+      <c r="B340" t="inlineStr"/>
+      <c r="C340" t="inlineStr"/>
+      <c r="D340" t="inlineStr"/>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr"/>
+      <c r="B341" t="inlineStr"/>
+      <c r="C341" t="inlineStr"/>
+      <c r="D341" t="inlineStr"/>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr"/>
+      <c r="B342" t="inlineStr"/>
+      <c r="C342" t="inlineStr"/>
+      <c r="D342" t="inlineStr"/>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr"/>
+      <c r="B343" t="inlineStr"/>
+      <c r="C343" t="inlineStr"/>
+      <c r="D343" t="inlineStr"/>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr"/>
+      <c r="B344" t="inlineStr"/>
+      <c r="C344" t="inlineStr"/>
+      <c r="D344" t="inlineStr"/>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr"/>
+      <c r="B345" t="inlineStr"/>
+      <c r="C345" t="inlineStr"/>
+      <c r="D345" t="inlineStr"/>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr"/>
+      <c r="B346" t="inlineStr"/>
+      <c r="C346" t="inlineStr"/>
+      <c r="D346" t="inlineStr"/>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr"/>
+      <c r="B347" t="inlineStr"/>
+      <c r="C347" t="inlineStr"/>
+      <c r="D347" t="inlineStr"/>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr"/>
+      <c r="B348" t="inlineStr"/>
+      <c r="C348" t="inlineStr"/>
+      <c r="D348" t="inlineStr"/>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr"/>
+      <c r="B349" t="inlineStr"/>
+      <c r="C349" t="inlineStr"/>
+      <c r="D349" t="inlineStr"/>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr"/>
+      <c r="B350" t="inlineStr"/>
+      <c r="C350" t="inlineStr"/>
+      <c r="D350" t="inlineStr"/>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr"/>
+      <c r="B351" t="inlineStr"/>
+      <c r="C351" t="inlineStr"/>
+      <c r="D351" t="inlineStr"/>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr"/>
+      <c r="B352" t="inlineStr"/>
+      <c r="C352" t="inlineStr"/>
+      <c r="D352" t="inlineStr"/>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr"/>
+      <c r="B353" t="inlineStr"/>
+      <c r="C353" t="inlineStr"/>
+      <c r="D353" t="inlineStr"/>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr"/>
+      <c r="B354" t="inlineStr"/>
+      <c r="C354" t="inlineStr"/>
+      <c r="D354" t="inlineStr"/>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr"/>
+      <c r="B355" t="inlineStr"/>
+      <c r="C355" t="inlineStr"/>
+      <c r="D355" t="inlineStr"/>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr"/>
+      <c r="B356" t="inlineStr"/>
+      <c r="C356" t="inlineStr"/>
+      <c r="D356" t="inlineStr"/>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr"/>
+      <c r="B357" t="inlineStr"/>
+      <c r="C357" t="inlineStr"/>
+      <c r="D357" t="inlineStr"/>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr"/>
+      <c r="B358" t="inlineStr"/>
+      <c r="C358" t="inlineStr"/>
+      <c r="D358" t="inlineStr"/>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr"/>
+      <c r="B359" t="inlineStr"/>
+      <c r="C359" t="inlineStr"/>
+      <c r="D359" t="inlineStr"/>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr"/>
+      <c r="B360" t="inlineStr"/>
+      <c r="C360" t="inlineStr"/>
+      <c r="D360" t="inlineStr"/>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr"/>
+      <c r="B361" t="inlineStr"/>
+      <c r="C361" t="inlineStr"/>
+      <c r="D361" t="inlineStr"/>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr"/>
+      <c r="B362" t="inlineStr"/>
+      <c r="C362" t="inlineStr"/>
+      <c r="D362" t="inlineStr"/>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr"/>
+      <c r="B363" t="inlineStr"/>
+      <c r="C363" t="inlineStr"/>
+      <c r="D363" t="inlineStr"/>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr"/>
+      <c r="B364" t="inlineStr"/>
+      <c r="C364" t="inlineStr"/>
+      <c r="D364" t="inlineStr"/>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr"/>
+      <c r="B365" t="inlineStr"/>
+      <c r="C365" t="inlineStr"/>
+      <c r="D365" t="inlineStr"/>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr"/>
+      <c r="B366" t="inlineStr"/>
+      <c r="C366" t="inlineStr"/>
+      <c r="D366" t="inlineStr"/>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr"/>
+      <c r="B367" t="inlineStr"/>
+      <c r="C367" t="inlineStr"/>
+      <c r="D367" t="inlineStr"/>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr"/>
+      <c r="B368" t="inlineStr"/>
+      <c r="C368" t="inlineStr"/>
+      <c r="D368" t="inlineStr"/>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr"/>
+      <c r="B369" t="inlineStr"/>
+      <c r="C369" t="inlineStr"/>
+      <c r="D369" t="inlineStr"/>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr"/>
+      <c r="B370" t="inlineStr"/>
+      <c r="C370" t="inlineStr"/>
+      <c r="D370" t="inlineStr"/>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr"/>
+      <c r="B371" t="inlineStr"/>
+      <c r="C371" t="inlineStr"/>
+      <c r="D371" t="inlineStr"/>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr"/>
+      <c r="B372" t="inlineStr"/>
+      <c r="C372" t="inlineStr"/>
+      <c r="D372" t="inlineStr"/>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr"/>
+      <c r="B373" t="inlineStr"/>
+      <c r="C373" t="inlineStr"/>
+      <c r="D373" t="inlineStr"/>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr"/>
+      <c r="B374" t="inlineStr"/>
+      <c r="C374" t="inlineStr"/>
+      <c r="D374" t="inlineStr"/>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr"/>
+      <c r="B375" t="inlineStr"/>
+      <c r="C375" t="inlineStr"/>
+      <c r="D375" t="inlineStr"/>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr"/>
+      <c r="B376" t="inlineStr"/>
+      <c r="C376" t="inlineStr"/>
+      <c r="D376" t="inlineStr"/>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr"/>
+      <c r="B377" t="inlineStr"/>
+      <c r="C377" t="inlineStr"/>
+      <c r="D377" t="inlineStr"/>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr"/>
+      <c r="B378" t="inlineStr"/>
+      <c r="C378" t="inlineStr"/>
+      <c r="D378" t="inlineStr"/>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr"/>
+      <c r="B379" t="inlineStr"/>
+      <c r="C379" t="inlineStr"/>
+      <c r="D379" t="inlineStr"/>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr"/>
+      <c r="B380" t="inlineStr"/>
+      <c r="C380" t="inlineStr"/>
+      <c r="D380" t="inlineStr"/>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr"/>
+      <c r="B381" t="inlineStr"/>
+      <c r="C381" t="inlineStr"/>
+      <c r="D381" t="inlineStr"/>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr"/>
+      <c r="B382" t="inlineStr"/>
+      <c r="C382" t="inlineStr"/>
+      <c r="D382" t="inlineStr"/>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr"/>
+      <c r="B383" t="inlineStr"/>
+      <c r="C383" t="inlineStr"/>
+      <c r="D383" t="inlineStr"/>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr"/>
+      <c r="B384" t="inlineStr"/>
+      <c r="C384" t="inlineStr"/>
+      <c r="D384" t="inlineStr"/>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr"/>
+      <c r="B385" t="inlineStr"/>
+      <c r="C385" t="inlineStr"/>
+      <c r="D385" t="inlineStr"/>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr"/>
+      <c r="B386" t="inlineStr"/>
+      <c r="C386" t="inlineStr"/>
+      <c r="D386" t="inlineStr"/>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr"/>
+      <c r="B387" t="inlineStr"/>
+      <c r="C387" t="inlineStr"/>
+      <c r="D387" t="inlineStr"/>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr"/>
+      <c r="B388" t="inlineStr"/>
+      <c r="C388" t="inlineStr"/>
+      <c r="D388" t="inlineStr"/>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr"/>
+      <c r="B389" t="inlineStr"/>
+      <c r="C389" t="inlineStr"/>
+      <c r="D389" t="inlineStr"/>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr"/>
+      <c r="B390" t="inlineStr"/>
+      <c r="C390" t="inlineStr"/>
+      <c r="D390" t="inlineStr"/>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr"/>
+      <c r="B391" t="inlineStr"/>
+      <c r="C391" t="inlineStr"/>
+      <c r="D391" t="inlineStr"/>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr"/>
+      <c r="B392" t="inlineStr"/>
+      <c r="C392" t="inlineStr"/>
+      <c r="D392" t="inlineStr"/>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr"/>
+      <c r="B393" t="inlineStr"/>
+      <c r="C393" t="inlineStr"/>
+      <c r="D393" t="inlineStr"/>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr"/>
+      <c r="B394" t="inlineStr"/>
+      <c r="C394" t="inlineStr"/>
+      <c r="D394" t="inlineStr"/>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr"/>
+      <c r="B395" t="inlineStr"/>
+      <c r="C395" t="inlineStr"/>
+      <c r="D395" t="inlineStr"/>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr"/>
+      <c r="B396" t="inlineStr"/>
+      <c r="C396" t="inlineStr"/>
+      <c r="D396" t="inlineStr"/>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr"/>
+      <c r="B397" t="inlineStr"/>
+      <c r="C397" t="inlineStr"/>
+      <c r="D397" t="inlineStr"/>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr"/>
+      <c r="B398" t="inlineStr"/>
+      <c r="C398" t="inlineStr"/>
+      <c r="D398" t="inlineStr"/>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr"/>
+      <c r="B399" t="inlineStr"/>
+      <c r="C399" t="inlineStr"/>
+      <c r="D399" t="inlineStr"/>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr"/>
+      <c r="B400" t="inlineStr"/>
+      <c r="C400" t="inlineStr"/>
+      <c r="D400" t="inlineStr"/>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr"/>
+      <c r="B401" t="inlineStr"/>
+      <c r="C401" t="inlineStr"/>
+      <c r="D401" t="inlineStr"/>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr"/>
+      <c r="B402" t="inlineStr"/>
+      <c r="C402" t="inlineStr"/>
+      <c r="D402" t="inlineStr"/>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr"/>
+      <c r="B403" t="inlineStr"/>
+      <c r="C403" t="inlineStr"/>
+      <c r="D403" t="inlineStr"/>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr"/>
+      <c r="B404" t="inlineStr"/>
+      <c r="C404" t="inlineStr"/>
+      <c r="D404" t="inlineStr"/>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr"/>
+      <c r="B405" t="inlineStr"/>
+      <c r="C405" t="inlineStr"/>
+      <c r="D405" t="inlineStr"/>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr"/>
+      <c r="B406" t="inlineStr"/>
+      <c r="C406" t="inlineStr"/>
+      <c r="D406" t="inlineStr"/>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr"/>
+      <c r="B407" t="inlineStr"/>
+      <c r="C407" t="inlineStr"/>
+      <c r="D407" t="inlineStr"/>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr"/>
+      <c r="B408" t="inlineStr"/>
+      <c r="C408" t="inlineStr"/>
+      <c r="D408" t="inlineStr"/>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr"/>
+      <c r="B409" t="inlineStr"/>
+      <c r="C409" t="inlineStr"/>
+      <c r="D409" t="inlineStr"/>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr"/>
+      <c r="B410" t="inlineStr"/>
+      <c r="C410" t="inlineStr"/>
+      <c r="D410" t="inlineStr"/>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr"/>
+      <c r="B411" t="inlineStr"/>
+      <c r="C411" t="inlineStr"/>
+      <c r="D411" t="inlineStr"/>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr"/>
+      <c r="B412" t="inlineStr"/>
+      <c r="C412" t="inlineStr"/>
+      <c r="D412" t="inlineStr"/>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr"/>
+      <c r="B413" t="inlineStr"/>
+      <c r="C413" t="inlineStr"/>
+      <c r="D413" t="inlineStr"/>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr"/>
+      <c r="B414" t="inlineStr"/>
+      <c r="C414" t="inlineStr"/>
+      <c r="D414" t="inlineStr"/>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr"/>
+      <c r="B415" t="inlineStr"/>
+      <c r="C415" t="inlineStr"/>
+      <c r="D415" t="inlineStr"/>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr"/>
+      <c r="B416" t="inlineStr"/>
+      <c r="C416" t="inlineStr"/>
+      <c r="D416" t="inlineStr"/>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr"/>
+      <c r="B417" t="inlineStr"/>
+      <c r="C417" t="inlineStr"/>
+      <c r="D417" t="inlineStr"/>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr"/>
+      <c r="B418" t="inlineStr"/>
+      <c r="C418" t="inlineStr"/>
+      <c r="D418" t="inlineStr"/>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr"/>
+      <c r="B419" t="inlineStr"/>
+      <c r="C419" t="inlineStr"/>
+      <c r="D419" t="inlineStr"/>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr"/>
+      <c r="B420" t="inlineStr"/>
+      <c r="C420" t="inlineStr"/>
+      <c r="D420" t="inlineStr"/>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr"/>
+      <c r="B421" t="inlineStr"/>
+      <c r="C421" t="inlineStr"/>
+      <c r="D421" t="inlineStr"/>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr"/>
+      <c r="B422" t="inlineStr"/>
+      <c r="C422" t="inlineStr"/>
+      <c r="D422" t="inlineStr"/>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr"/>
+      <c r="B423" t="inlineStr"/>
+      <c r="C423" t="inlineStr"/>
+      <c r="D423" t="inlineStr"/>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr"/>
+      <c r="B424" t="inlineStr"/>
+      <c r="C424" t="inlineStr"/>
+      <c r="D424" t="inlineStr"/>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr"/>
+      <c r="B425" t="inlineStr"/>
+      <c r="C425" t="inlineStr"/>
+      <c r="D425" t="inlineStr"/>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr"/>
+      <c r="B426" t="inlineStr"/>
+      <c r="C426" t="inlineStr"/>
+      <c r="D426" t="inlineStr"/>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr"/>
+      <c r="B427" t="inlineStr"/>
+      <c r="C427" t="inlineStr"/>
+      <c r="D427" t="inlineStr"/>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr"/>
+      <c r="B428" t="inlineStr"/>
+      <c r="C428" t="inlineStr"/>
+      <c r="D428" t="inlineStr"/>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr"/>
+      <c r="B429" t="inlineStr"/>
+      <c r="C429" t="inlineStr"/>
+      <c r="D429" t="inlineStr"/>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr"/>
+      <c r="B430" t="inlineStr"/>
+      <c r="C430" t="inlineStr"/>
+      <c r="D430" t="inlineStr"/>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr"/>
+      <c r="B431" t="inlineStr"/>
+      <c r="C431" t="inlineStr"/>
+      <c r="D431" t="inlineStr"/>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr"/>
+      <c r="B432" t="inlineStr"/>
+      <c r="C432" t="inlineStr"/>
+      <c r="D432" t="inlineStr"/>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr"/>
+      <c r="B433" t="inlineStr"/>
+      <c r="C433" t="inlineStr"/>
+      <c r="D433" t="inlineStr"/>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr"/>
+      <c r="B434" t="inlineStr"/>
+      <c r="C434" t="inlineStr"/>
+      <c r="D434" t="inlineStr"/>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr"/>
+      <c r="B435" t="inlineStr"/>
+      <c r="C435" t="inlineStr"/>
+      <c r="D435" t="inlineStr"/>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr"/>
+      <c r="B436" t="inlineStr"/>
+      <c r="C436" t="inlineStr"/>
+      <c r="D436" t="inlineStr"/>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr"/>
+      <c r="B437" t="inlineStr"/>
+      <c r="C437" t="inlineStr"/>
+      <c r="D437" t="inlineStr"/>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr"/>
+      <c r="B438" t="inlineStr"/>
+      <c r="C438" t="inlineStr"/>
+      <c r="D438" t="inlineStr"/>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr"/>
+      <c r="B439" t="inlineStr"/>
+      <c r="C439" t="inlineStr"/>
+      <c r="D439" t="inlineStr"/>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr"/>
+      <c r="B440" t="inlineStr"/>
+      <c r="C440" t="inlineStr"/>
+      <c r="D440" t="inlineStr"/>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr"/>
+      <c r="B441" t="inlineStr"/>
+      <c r="C441" t="inlineStr"/>
+      <c r="D441" t="inlineStr"/>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr"/>
+      <c r="B442" t="inlineStr"/>
+      <c r="C442" t="inlineStr"/>
+      <c r="D442" t="inlineStr"/>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr"/>
+      <c r="B443" t="inlineStr"/>
+      <c r="C443" t="inlineStr"/>
+      <c r="D443" t="inlineStr"/>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr"/>
+      <c r="B444" t="inlineStr"/>
+      <c r="C444" t="inlineStr"/>
+      <c r="D444" t="inlineStr"/>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr"/>
+      <c r="B445" t="inlineStr"/>
+      <c r="C445" t="inlineStr"/>
+      <c r="D445" t="inlineStr"/>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr"/>
+      <c r="B446" t="inlineStr"/>
+      <c r="C446" t="inlineStr"/>
+      <c r="D446" t="inlineStr"/>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr"/>
+      <c r="B447" t="inlineStr"/>
+      <c r="C447" t="inlineStr"/>
+      <c r="D447" t="inlineStr"/>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr"/>
+      <c r="B448" t="inlineStr"/>
+      <c r="C448" t="inlineStr"/>
+      <c r="D448" t="inlineStr"/>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr"/>
+      <c r="B449" t="inlineStr"/>
+      <c r="C449" t="inlineStr"/>
+      <c r="D449" t="inlineStr"/>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr"/>
+      <c r="B450" t="inlineStr"/>
+      <c r="C450" t="inlineStr"/>
+      <c r="D450" t="inlineStr"/>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr"/>
+      <c r="B451" t="inlineStr"/>
+      <c r="C451" t="inlineStr"/>
+      <c r="D451" t="inlineStr"/>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr"/>
+      <c r="B452" t="inlineStr"/>
+      <c r="C452" t="inlineStr"/>
+      <c r="D452" t="inlineStr"/>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr"/>
+      <c r="B453" t="inlineStr"/>
+      <c r="C453" t="inlineStr"/>
+      <c r="D453" t="inlineStr"/>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr"/>
+      <c r="B454" t="inlineStr"/>
+      <c r="C454" t="inlineStr"/>
+      <c r="D454" t="inlineStr"/>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr"/>
+      <c r="B455" t="inlineStr"/>
+      <c r="C455" t="inlineStr"/>
+      <c r="D455" t="inlineStr"/>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr"/>
+      <c r="B456" t="inlineStr"/>
+      <c r="C456" t="inlineStr"/>
+      <c r="D456" t="inlineStr"/>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr"/>
+      <c r="B457" t="inlineStr"/>
+      <c r="C457" t="inlineStr"/>
+      <c r="D457" t="inlineStr"/>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr"/>
+      <c r="B458" t="inlineStr"/>
+      <c r="C458" t="inlineStr"/>
+      <c r="D458" t="inlineStr"/>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr"/>
+      <c r="B459" t="inlineStr"/>
+      <c r="C459" t="inlineStr"/>
+      <c r="D459" t="inlineStr"/>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr"/>
+      <c r="B460" t="inlineStr"/>
+      <c r="C460" t="inlineStr"/>
+      <c r="D460" t="inlineStr"/>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr"/>
+      <c r="B461" t="inlineStr"/>
+      <c r="C461" t="inlineStr"/>
+      <c r="D461" t="inlineStr"/>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr"/>
+      <c r="B462" t="inlineStr"/>
+      <c r="C462" t="inlineStr"/>
+      <c r="D462" t="inlineStr"/>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr"/>
+      <c r="B463" t="inlineStr"/>
+      <c r="C463" t="inlineStr"/>
+      <c r="D463" t="inlineStr"/>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr"/>
+      <c r="B464" t="inlineStr"/>
+      <c r="C464" t="inlineStr"/>
+      <c r="D464" t="inlineStr"/>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr"/>
+      <c r="B465" t="inlineStr"/>
+      <c r="C465" t="inlineStr"/>
+      <c r="D465" t="inlineStr"/>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr"/>
+      <c r="B466" t="inlineStr"/>
+      <c r="C466" t="inlineStr"/>
+      <c r="D466" t="inlineStr"/>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr"/>
+      <c r="B467" t="inlineStr"/>
+      <c r="C467" t="inlineStr"/>
+      <c r="D467" t="inlineStr"/>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr"/>
+      <c r="B468" t="inlineStr"/>
+      <c r="C468" t="inlineStr"/>
+      <c r="D468" t="inlineStr"/>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr"/>
+      <c r="B469" t="inlineStr"/>
+      <c r="C469" t="inlineStr"/>
+      <c r="D469" t="inlineStr"/>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr"/>
+      <c r="B470" t="inlineStr"/>
+      <c r="C470" t="inlineStr"/>
+      <c r="D470" t="inlineStr"/>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr"/>
+      <c r="B471" t="inlineStr"/>
+      <c r="C471" t="inlineStr"/>
+      <c r="D471" t="inlineStr"/>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr"/>
+      <c r="B472" t="inlineStr"/>
+      <c r="C472" t="inlineStr"/>
+      <c r="D472" t="inlineStr"/>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr"/>
+      <c r="B473" t="inlineStr"/>
+      <c r="C473" t="inlineStr"/>
+      <c r="D473" t="inlineStr"/>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr"/>
+      <c r="B474" t="inlineStr"/>
+      <c r="C474" t="inlineStr"/>
+      <c r="D474" t="inlineStr"/>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr"/>
+      <c r="B475" t="inlineStr"/>
+      <c r="C475" t="inlineStr"/>
+      <c r="D475" t="inlineStr"/>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr"/>
+      <c r="B476" t="inlineStr"/>
+      <c r="C476" t="inlineStr"/>
+      <c r="D476" t="inlineStr"/>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr"/>
+      <c r="B477" t="inlineStr"/>
+      <c r="C477" t="inlineStr"/>
+      <c r="D477" t="inlineStr"/>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr"/>
+      <c r="B478" t="inlineStr"/>
+      <c r="C478" t="inlineStr"/>
+      <c r="D478" t="inlineStr"/>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr"/>
+      <c r="B479" t="inlineStr"/>
+      <c r="C479" t="inlineStr"/>
+      <c r="D479" t="inlineStr"/>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr"/>
+      <c r="B480" t="inlineStr"/>
+      <c r="C480" t="inlineStr"/>
+      <c r="D480" t="inlineStr"/>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr"/>
+      <c r="B481" t="inlineStr"/>
+      <c r="C481" t="inlineStr"/>
+      <c r="D481" t="inlineStr"/>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr"/>
+      <c r="B482" t="inlineStr"/>
+      <c r="C482" t="inlineStr"/>
+      <c r="D482" t="inlineStr"/>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr"/>
+      <c r="B483" t="inlineStr"/>
+      <c r="C483" t="inlineStr"/>
+      <c r="D483" t="inlineStr"/>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr"/>
+      <c r="B484" t="inlineStr"/>
+      <c r="C484" t="inlineStr"/>
+      <c r="D484" t="inlineStr"/>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr"/>
+      <c r="B485" t="inlineStr"/>
+      <c r="C485" t="inlineStr"/>
+      <c r="D485" t="inlineStr"/>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr"/>
+      <c r="B486" t="inlineStr"/>
+      <c r="C486" t="inlineStr"/>
+      <c r="D486" t="inlineStr"/>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr"/>
+      <c r="B487" t="inlineStr"/>
+      <c r="C487" t="inlineStr"/>
+      <c r="D487" t="inlineStr"/>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr"/>
+      <c r="B488" t="inlineStr"/>
+      <c r="C488" t="inlineStr"/>
+      <c r="D488" t="inlineStr"/>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr"/>
+      <c r="B489" t="inlineStr"/>
+      <c r="C489" t="inlineStr"/>
+      <c r="D489" t="inlineStr"/>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr"/>
+      <c r="B490" t="inlineStr"/>
+      <c r="C490" t="inlineStr"/>
+      <c r="D490" t="inlineStr"/>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr"/>
+      <c r="B491" t="inlineStr"/>
+      <c r="C491" t="inlineStr"/>
+      <c r="D491" t="inlineStr"/>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr"/>
+      <c r="B492" t="inlineStr"/>
+      <c r="C492" t="inlineStr"/>
+      <c r="D492" t="inlineStr"/>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr"/>
+      <c r="B493" t="inlineStr"/>
+      <c r="C493" t="inlineStr"/>
+      <c r="D493" t="inlineStr"/>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr"/>
+      <c r="B494" t="inlineStr"/>
+      <c r="C494" t="inlineStr"/>
+      <c r="D494" t="inlineStr"/>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr"/>
+      <c r="B495" t="inlineStr"/>
+      <c r="C495" t="inlineStr"/>
+      <c r="D495" t="inlineStr"/>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr"/>
+      <c r="B496" t="inlineStr"/>
+      <c r="C496" t="inlineStr"/>
+      <c r="D496" t="inlineStr"/>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr"/>
+      <c r="B497" t="inlineStr"/>
+      <c r="C497" t="inlineStr"/>
+      <c r="D497" t="inlineStr"/>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr"/>
+      <c r="B498" t="inlineStr"/>
+      <c r="C498" t="inlineStr"/>
+      <c r="D498" t="inlineStr"/>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr"/>
+      <c r="B499" t="inlineStr"/>
+      <c r="C499" t="inlineStr"/>
+      <c r="D499" t="inlineStr"/>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr"/>
+      <c r="B500" t="inlineStr"/>
+      <c r="C500" t="inlineStr"/>
+      <c r="D500" t="inlineStr"/>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr"/>
+      <c r="B501" t="inlineStr"/>
+      <c r="C501" t="inlineStr"/>
+      <c r="D501" t="n">
+        <v>392296156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>